<commit_message>
little fix so we can have custom event names persist
</commit_message>
<xml_diff>
--- a/seeds/Formulaic Seed generation.xlsx
+++ b/seeds/Formulaic Seed generation.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reeveschragger/Documents/Bootcamp/Projects/Farmers-Market-Organiser/seeds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DEDD53E4-A58C-0144-9E47-8A70AA9D2A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB8D098-B809-FE4A-87CE-BAE3BA0DB90D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{E72EE37F-B9BE-8B4C-AF7C-D3608E94063D}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16400" activeTab="1" xr2:uid="{E72EE37F-B9BE-8B4C-AF7C-D3608E94063D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Stall" sheetId="1" r:id="rId1"/>
+    <sheet name="Event" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="65">
   <si>
     <t>stall_name</t>
   </si>
@@ -224,13 +225,23 @@
   </si>
   <si>
     <t>IceCream Van</t>
+  </si>
+  <si>
+    <t>timestamp_start</t>
+  </si>
+  <si>
+    <t>timestamp_end</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="171" formatCode="[$-C09]dddd\,\ d/m/yyyy;@"/>
+    <numFmt numFmtId="172" formatCode="[$-409]h:mm:ss\ am/pm;@"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -243,6 +254,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF001080"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -271,9 +288,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80609DE7-2449-714B-A221-516362804272}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D14" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1205,4 +1226,948 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A42D5DFB-A5D4-CF45-89DE-E7557FAEE80C}">
+  <dimension ref="A1:G41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="str">
+        <f>TEXT(E2,"DD/MM/YYYY") &amp; " " &amp; TEXT(F2,"H:MM")</f>
+        <v>01/09/2022 9:00</v>
+      </c>
+      <c r="C2" t="str">
+        <f>TEXT(E2,"DD/MM/YYYY") &amp; " " &amp; TEXT(G2,"H:MM")</f>
+        <v>01/09/2022 15:00</v>
+      </c>
+      <c r="E2" s="4">
+        <v>44805</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="str">
+        <f t="shared" ref="B3:B41" si="0">TEXT(E3,"DD/MM/YYYY") &amp; " " &amp; TEXT(F3,"H:MM")</f>
+        <v>02/09/2022 9:00</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C41" si="1">TEXT(E3,"DD/MM/YYYY") &amp; " " &amp; TEXT(G3,"H:MM")</f>
+        <v>02/09/2022 15:00</v>
+      </c>
+      <c r="E3" s="4">
+        <v>44806</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>03/09/2022 9:00</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="1"/>
+        <v>03/09/2022 15:00</v>
+      </c>
+      <c r="E4" s="4">
+        <v>44807</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>04/09/2022 9:00</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="1"/>
+        <v>04/09/2022 15:00</v>
+      </c>
+      <c r="E5" s="4">
+        <v>44808</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>08/09/2022 9:00</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="1"/>
+        <v>08/09/2022 15:00</v>
+      </c>
+      <c r="E6" s="4">
+        <f>E2+7</f>
+        <v>44812</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>09/09/2022 9:00</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="1"/>
+        <v>09/09/2022 15:00</v>
+      </c>
+      <c r="E7" s="4">
+        <f>E6+1</f>
+        <v>44813</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>10/09/2022 9:00</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="1"/>
+        <v>10/09/2022 15:00</v>
+      </c>
+      <c r="E8" s="4">
+        <f t="shared" ref="E8:E17" si="2">E7+1</f>
+        <v>44814</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>1</v>
+      </c>
+      <c r="B9" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>11/09/2022 9:00</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="1"/>
+        <v>11/09/2022 15:00</v>
+      </c>
+      <c r="E9" s="4">
+        <f t="shared" si="2"/>
+        <v>44815</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>1</v>
+      </c>
+      <c r="B10" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>15/09/2022 9:00</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="1"/>
+        <v>15/09/2022 15:00</v>
+      </c>
+      <c r="E10" s="4">
+        <f>E6+7</f>
+        <v>44819</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>16/09/2022 9:00</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="1"/>
+        <v>16/09/2022 15:00</v>
+      </c>
+      <c r="E11" s="4">
+        <f>E10+1</f>
+        <v>44820</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>1</v>
+      </c>
+      <c r="B12" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>17/09/2022 9:00</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="1"/>
+        <v>17/09/2022 15:00</v>
+      </c>
+      <c r="E12" s="4">
+        <f t="shared" ref="E12:E21" si="3">E11+1</f>
+        <v>44821</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>1</v>
+      </c>
+      <c r="B13" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>18/09/2022 9:00</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="1"/>
+        <v>18/09/2022 15:00</v>
+      </c>
+      <c r="E13" s="4">
+        <f t="shared" si="3"/>
+        <v>44822</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>1</v>
+      </c>
+      <c r="B14" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>22/09/2022 9:00</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="1"/>
+        <v>22/09/2022 15:00</v>
+      </c>
+      <c r="E14" s="4">
+        <f>E10+7</f>
+        <v>44826</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>1</v>
+      </c>
+      <c r="B15" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>23/09/2022 9:00</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="1"/>
+        <v>23/09/2022 15:00</v>
+      </c>
+      <c r="E15" s="4">
+        <f>E14+1</f>
+        <v>44827</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>1</v>
+      </c>
+      <c r="B16" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>24/09/2022 9:00</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="1"/>
+        <v>24/09/2022 15:00</v>
+      </c>
+      <c r="E16" s="4">
+        <f t="shared" ref="E16:E21" si="4">E15+1</f>
+        <v>44828</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>1</v>
+      </c>
+      <c r="B17" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>25/09/2022 9:00</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="1"/>
+        <v>25/09/2022 15:00</v>
+      </c>
+      <c r="E17" s="4">
+        <f t="shared" si="4"/>
+        <v>44829</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>1</v>
+      </c>
+      <c r="B18" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>29/09/2022 9:00</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="1"/>
+        <v>29/09/2022 15:00</v>
+      </c>
+      <c r="E18" s="4">
+        <f>E14+7</f>
+        <v>44833</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>1</v>
+      </c>
+      <c r="B19" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>30/09/2022 9:00</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="1"/>
+        <v>30/09/2022 15:00</v>
+      </c>
+      <c r="E19" s="4">
+        <f>E18+1</f>
+        <v>44834</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>1</v>
+      </c>
+      <c r="B20" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>01/10/2022 9:00</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="1"/>
+        <v>01/10/2022 15:00</v>
+      </c>
+      <c r="E20" s="4">
+        <f t="shared" ref="E20:E21" si="5">E19+1</f>
+        <v>44835</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>1</v>
+      </c>
+      <c r="B21" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>02/10/2022 9:00</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="1"/>
+        <v>02/10/2022 15:00</v>
+      </c>
+      <c r="E21" s="4">
+        <f t="shared" si="5"/>
+        <v>44836</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>01/09/2022 8:00</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="1"/>
+        <v>01/09/2022 13:30</v>
+      </c>
+      <c r="E22" s="4">
+        <v>44805</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>02/09/2022 8:00</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="1"/>
+        <v>02/09/2022 13:30</v>
+      </c>
+      <c r="E23" s="4">
+        <v>44806</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>03/09/2022 8:00</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="1"/>
+        <v>03/09/2022 13:30</v>
+      </c>
+      <c r="E24" s="4">
+        <v>44807</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G24" s="3">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>04/09/2022 8:00</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="1"/>
+        <v>04/09/2022 13:30</v>
+      </c>
+      <c r="E25" s="4">
+        <v>44808</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G25" s="3">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>08/09/2022 8:00</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="1"/>
+        <v>08/09/2022 13:30</v>
+      </c>
+      <c r="E26" s="4">
+        <f>E22+7</f>
+        <v>44812</v>
+      </c>
+      <c r="F26" s="3">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>09/09/2022 8:00</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="1"/>
+        <v>09/09/2022 13:30</v>
+      </c>
+      <c r="E27" s="4">
+        <f>E26+1</f>
+        <v>44813</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="B28" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>10/09/2022 8:00</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="1"/>
+        <v>10/09/2022 13:30</v>
+      </c>
+      <c r="E28" s="4">
+        <f t="shared" ref="E28:E37" si="6">E27+1</f>
+        <v>44814</v>
+      </c>
+      <c r="F28" s="3">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>11/09/2022 8:00</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="1"/>
+        <v>11/09/2022 13:30</v>
+      </c>
+      <c r="E29" s="4">
+        <f t="shared" si="6"/>
+        <v>44815</v>
+      </c>
+      <c r="F29" s="3">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>15/09/2022 8:00</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="1"/>
+        <v>15/09/2022 13:30</v>
+      </c>
+      <c r="E30" s="4">
+        <f>E26+7</f>
+        <v>44819</v>
+      </c>
+      <c r="F30" s="3">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G30" s="3">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>16/09/2022 8:00</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="1"/>
+        <v>16/09/2022 13:30</v>
+      </c>
+      <c r="E31" s="4">
+        <f>E30+1</f>
+        <v>44820</v>
+      </c>
+      <c r="F31" s="3">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G31" s="3">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>2</v>
+      </c>
+      <c r="B32" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>17/09/2022 8:00</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="1"/>
+        <v>17/09/2022 13:30</v>
+      </c>
+      <c r="E32" s="4">
+        <f t="shared" ref="E32:E41" si="7">E31+1</f>
+        <v>44821</v>
+      </c>
+      <c r="F32" s="3">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G32" s="3">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>2</v>
+      </c>
+      <c r="B33" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>18/09/2022 8:00</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="1"/>
+        <v>18/09/2022 13:30</v>
+      </c>
+      <c r="E33" s="4">
+        <f t="shared" si="7"/>
+        <v>44822</v>
+      </c>
+      <c r="F33" s="3">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G33" s="3">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>2</v>
+      </c>
+      <c r="B34" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>22/09/2022 8:00</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="1"/>
+        <v>22/09/2022 13:30</v>
+      </c>
+      <c r="E34" s="4">
+        <f>E30+7</f>
+        <v>44826</v>
+      </c>
+      <c r="F34" s="3">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G34" s="3">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>2</v>
+      </c>
+      <c r="B35" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>23/09/2022 8:00</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="1"/>
+        <v>23/09/2022 13:30</v>
+      </c>
+      <c r="E35" s="4">
+        <f>E34+1</f>
+        <v>44827</v>
+      </c>
+      <c r="F35" s="3">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G35" s="3">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>2</v>
+      </c>
+      <c r="B36" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>24/09/2022 8:00</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="1"/>
+        <v>24/09/2022 13:30</v>
+      </c>
+      <c r="E36" s="4">
+        <f t="shared" ref="E36:E41" si="8">E35+1</f>
+        <v>44828</v>
+      </c>
+      <c r="F36" s="3">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G36" s="3">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>2</v>
+      </c>
+      <c r="B37" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>25/09/2022 8:00</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="1"/>
+        <v>25/09/2022 13:30</v>
+      </c>
+      <c r="E37" s="4">
+        <f t="shared" si="8"/>
+        <v>44829</v>
+      </c>
+      <c r="F37" s="3">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G37" s="3">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>2</v>
+      </c>
+      <c r="B38" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>29/09/2022 8:00</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="1"/>
+        <v>29/09/2022 13:30</v>
+      </c>
+      <c r="E38" s="4">
+        <f>E34+7</f>
+        <v>44833</v>
+      </c>
+      <c r="F38" s="3">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G38" s="3">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>2</v>
+      </c>
+      <c r="B39" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>30/09/2022 8:00</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="1"/>
+        <v>30/09/2022 13:30</v>
+      </c>
+      <c r="E39" s="4">
+        <f>E38+1</f>
+        <v>44834</v>
+      </c>
+      <c r="F39" s="3">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G39" s="3">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>2</v>
+      </c>
+      <c r="B40" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>01/10/2022 8:00</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="1"/>
+        <v>01/10/2022 13:30</v>
+      </c>
+      <c r="E40" s="4">
+        <f t="shared" ref="E40:E41" si="9">E39+1</f>
+        <v>44835</v>
+      </c>
+      <c r="F40" s="3">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G40" s="3">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>2</v>
+      </c>
+      <c r="B41" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>02/10/2022 8:00</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="1"/>
+        <v>02/10/2022 13:30</v>
+      </c>
+      <c r="E41" s="4">
+        <f t="shared" si="9"/>
+        <v>44836</v>
+      </c>
+      <c r="F41" s="3">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G41" s="3">
+        <v>0.5625</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Made changes to seed data to make 3 locations with different types of open days - 4 days a week, 2 days a week and first Sunday of the month. Also made some simple logos in
</commit_message>
<xml_diff>
--- a/seeds/Formulaic Seed generation.xlsx
+++ b/seeds/Formulaic Seed generation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reeveschragger/Documents/Bootcamp/Projects/Farmers-Market-Organiser/seeds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB8D098-B809-FE4A-87CE-BAE3BA0DB90D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0D6663-B6D6-C242-B615-A5AD156A5665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16400" activeTab="1" xr2:uid="{E72EE37F-B9BE-8B4C-AF7C-D3608E94063D}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16340" activeTab="1" xr2:uid="{E72EE37F-B9BE-8B4C-AF7C-D3608E94063D}"/>
   </bookViews>
   <sheets>
     <sheet name="Stall" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="68">
   <si>
     <t>stall_name</t>
   </si>
@@ -231,6 +231,15 @@
   </si>
   <si>
     <t>timestamp_end</t>
+  </si>
+  <si>
+    <t>CENTRAL 1</t>
+  </si>
+  <si>
+    <t>Southern 2</t>
+  </si>
+  <si>
+    <t>Eastern 3</t>
   </si>
 </sst>
 </file>
@@ -288,13 +297,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1230,10 +1242,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A42D5DFB-A5D4-CF45-89DE-E7557FAEE80C}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C41"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1241,10 +1253,10 @@
     <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1255,916 +1267,1043 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="str">
-        <f>TEXT(E2,"DD/MM/YYYY") &amp; " " &amp; TEXT(F2,"H:MM")</f>
+      <c r="B2" s="6" t="str">
+        <f>TEXT(F2,"DD/MM/YYYY") &amp; " " &amp; TEXT(G2,"H:MM")</f>
         <v>01/09/2022 9:00</v>
       </c>
-      <c r="C2" t="str">
-        <f>TEXT(E2,"DD/MM/YYYY") &amp; " " &amp; TEXT(G2,"H:MM")</f>
+      <c r="C2" s="1" t="str">
+        <f>TEXT(F2,"DD/MM/YYYY") &amp; " " &amp; TEXT(H2,"H:MM")</f>
         <v>01/09/2022 15:00</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="7">
         <v>44805</v>
       </c>
-      <c r="F2" s="3">
+      <c r="G2" s="8">
         <v>0.375</v>
       </c>
-      <c r="G2" s="3">
+      <c r="H2" s="8">
         <v>0.625</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="str">
-        <f t="shared" ref="B3:B41" si="0">TEXT(E3,"DD/MM/YYYY") &amp; " " &amp; TEXT(F3,"H:MM")</f>
+      <c r="B3" s="6" t="str">
+        <f>TEXT(F3,"DD/MM/YYYY") &amp; " " &amp; TEXT(G3,"H:MM")</f>
         <v>02/09/2022 9:00</v>
       </c>
-      <c r="C3" t="str">
-        <f t="shared" ref="C3:C41" si="1">TEXT(E3,"DD/MM/YYYY") &amp; " " &amp; TEXT(G3,"H:MM")</f>
+      <c r="C3" s="1" t="str">
+        <f>TEXT(F3,"DD/MM/YYYY") &amp; " " &amp; TEXT(H3,"H:MM")</f>
         <v>02/09/2022 15:00</v>
       </c>
-      <c r="E3" s="4">
+      <c r="F3" s="7">
         <v>44806</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G3" s="8">
         <v>0.375</v>
       </c>
-      <c r="G3" s="3">
+      <c r="H3" s="8">
         <v>0.625</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="5" t="str">
+      <c r="B4" s="6" t="str">
+        <f>TEXT(F4,"DD/MM/YYYY") &amp; " " &amp; TEXT(G4,"H:MM")</f>
+        <v>03/09/2022 9:00</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <f>TEXT(F4,"DD/MM/YYYY") &amp; " " &amp; TEXT(H4,"H:MM")</f>
+        <v>03/09/2022 15:00</v>
+      </c>
+      <c r="F4" s="7">
+        <v>44807</v>
+      </c>
+      <c r="G4" s="8">
+        <v>0.375</v>
+      </c>
+      <c r="H4" s="8">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="6" t="str">
+        <f>TEXT(F5,"DD/MM/YYYY") &amp; " " &amp; TEXT(G5,"H:MM")</f>
+        <v>04/09/2022 9:00</v>
+      </c>
+      <c r="C5" s="1" t="str">
+        <f>TEXT(F5,"DD/MM/YYYY") &amp; " " &amp; TEXT(H5,"H:MM")</f>
+        <v>04/09/2022 15:00</v>
+      </c>
+      <c r="F5" s="7">
+        <v>44808</v>
+      </c>
+      <c r="G5" s="8">
+        <v>0.375</v>
+      </c>
+      <c r="H5" s="8">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="6" t="str">
+        <f>TEXT(F6,"DD/MM/YYYY") &amp; " " &amp; TEXT(G6,"H:MM")</f>
+        <v>08/09/2022 9:00</v>
+      </c>
+      <c r="C6" s="1" t="str">
+        <f>TEXT(F6,"DD/MM/YYYY") &amp; " " &amp; TEXT(H6,"H:MM")</f>
+        <v>08/09/2022 15:00</v>
+      </c>
+      <c r="F6" s="7">
+        <f>F2+7</f>
+        <v>44812</v>
+      </c>
+      <c r="G6" s="8">
+        <v>0.375</v>
+      </c>
+      <c r="H6" s="8">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" s="6" t="str">
+        <f>TEXT(F7,"DD/MM/YYYY") &amp; " " &amp; TEXT(G7,"H:MM")</f>
+        <v>09/09/2022 9:00</v>
+      </c>
+      <c r="C7" s="1" t="str">
+        <f>TEXT(F7,"DD/MM/YYYY") &amp; " " &amp; TEXT(H7,"H:MM")</f>
+        <v>09/09/2022 15:00</v>
+      </c>
+      <c r="F7" s="7">
+        <f>F6+1</f>
+        <v>44813</v>
+      </c>
+      <c r="G7" s="8">
+        <v>0.375</v>
+      </c>
+      <c r="H7" s="8">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" s="6" t="str">
+        <f>TEXT(F8,"DD/MM/YYYY") &amp; " " &amp; TEXT(G8,"H:MM")</f>
+        <v>10/09/2022 9:00</v>
+      </c>
+      <c r="C8" s="1" t="str">
+        <f>TEXT(F8,"DD/MM/YYYY") &amp; " " &amp; TEXT(H8,"H:MM")</f>
+        <v>10/09/2022 15:00</v>
+      </c>
+      <c r="F8" s="7">
+        <f t="shared" ref="F8:F17" si="0">F7+1</f>
+        <v>44814</v>
+      </c>
+      <c r="G8" s="8">
+        <v>0.375</v>
+      </c>
+      <c r="H8" s="8">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>1</v>
+      </c>
+      <c r="B9" s="6" t="str">
+        <f>TEXT(F9,"DD/MM/YYYY") &amp; " " &amp; TEXT(G9,"H:MM")</f>
+        <v>11/09/2022 9:00</v>
+      </c>
+      <c r="C9" s="1" t="str">
+        <f>TEXT(F9,"DD/MM/YYYY") &amp; " " &amp; TEXT(H9,"H:MM")</f>
+        <v>11/09/2022 15:00</v>
+      </c>
+      <c r="F9" s="7">
         <f t="shared" si="0"/>
-        <v>03/09/2022 9:00</v>
-      </c>
-      <c r="C4" t="str">
+        <v>44815</v>
+      </c>
+      <c r="G9" s="8">
+        <v>0.375</v>
+      </c>
+      <c r="H9" s="8">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>1</v>
+      </c>
+      <c r="B10" s="6" t="str">
+        <f>TEXT(F10,"DD/MM/YYYY") &amp; " " &amp; TEXT(G10,"H:MM")</f>
+        <v>15/09/2022 9:00</v>
+      </c>
+      <c r="C10" s="1" t="str">
+        <f>TEXT(F10,"DD/MM/YYYY") &amp; " " &amp; TEXT(H10,"H:MM")</f>
+        <v>15/09/2022 15:00</v>
+      </c>
+      <c r="F10" s="7">
+        <f>F6+7</f>
+        <v>44819</v>
+      </c>
+      <c r="G10" s="8">
+        <v>0.375</v>
+      </c>
+      <c r="H10" s="8">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="6" t="str">
+        <f>TEXT(F11,"DD/MM/YYYY") &amp; " " &amp; TEXT(G11,"H:MM")</f>
+        <v>16/09/2022 9:00</v>
+      </c>
+      <c r="C11" s="1" t="str">
+        <f>TEXT(F11,"DD/MM/YYYY") &amp; " " &amp; TEXT(H11,"H:MM")</f>
+        <v>16/09/2022 15:00</v>
+      </c>
+      <c r="F11" s="7">
+        <f>F10+1</f>
+        <v>44820</v>
+      </c>
+      <c r="G11" s="8">
+        <v>0.375</v>
+      </c>
+      <c r="H11" s="8">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>1</v>
+      </c>
+      <c r="B12" s="6" t="str">
+        <f>TEXT(F12,"DD/MM/YYYY") &amp; " " &amp; TEXT(G12,"H:MM")</f>
+        <v>17/09/2022 9:00</v>
+      </c>
+      <c r="C12" s="1" t="str">
+        <f>TEXT(F12,"DD/MM/YYYY") &amp; " " &amp; TEXT(H12,"H:MM")</f>
+        <v>17/09/2022 15:00</v>
+      </c>
+      <c r="F12" s="7">
+        <f t="shared" ref="F12:F21" si="1">F11+1</f>
+        <v>44821</v>
+      </c>
+      <c r="G12" s="8">
+        <v>0.375</v>
+      </c>
+      <c r="H12" s="8">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>1</v>
+      </c>
+      <c r="B13" s="6" t="str">
+        <f>TEXT(F13,"DD/MM/YYYY") &amp; " " &amp; TEXT(G13,"H:MM")</f>
+        <v>18/09/2022 9:00</v>
+      </c>
+      <c r="C13" s="1" t="str">
+        <f>TEXT(F13,"DD/MM/YYYY") &amp; " " &amp; TEXT(H13,"H:MM")</f>
+        <v>18/09/2022 15:00</v>
+      </c>
+      <c r="F13" s="7">
         <f t="shared" si="1"/>
-        <v>03/09/2022 15:00</v>
-      </c>
-      <c r="E4" s="4">
+        <v>44822</v>
+      </c>
+      <c r="G13" s="8">
+        <v>0.375</v>
+      </c>
+      <c r="H13" s="8">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>1</v>
+      </c>
+      <c r="B14" s="6" t="str">
+        <f>TEXT(F14,"DD/MM/YYYY") &amp; " " &amp; TEXT(G14,"H:MM")</f>
+        <v>22/09/2022 9:00</v>
+      </c>
+      <c r="C14" s="1" t="str">
+        <f>TEXT(F14,"DD/MM/YYYY") &amp; " " &amp; TEXT(H14,"H:MM")</f>
+        <v>22/09/2022 15:00</v>
+      </c>
+      <c r="F14" s="7">
+        <f>F10+7</f>
+        <v>44826</v>
+      </c>
+      <c r="G14" s="8">
+        <v>0.375</v>
+      </c>
+      <c r="H14" s="8">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>1</v>
+      </c>
+      <c r="B15" s="6" t="str">
+        <f>TEXT(F15,"DD/MM/YYYY") &amp; " " &amp; TEXT(G15,"H:MM")</f>
+        <v>23/09/2022 9:00</v>
+      </c>
+      <c r="C15" s="1" t="str">
+        <f>TEXT(F15,"DD/MM/YYYY") &amp; " " &amp; TEXT(H15,"H:MM")</f>
+        <v>23/09/2022 15:00</v>
+      </c>
+      <c r="F15" s="7">
+        <f>F14+1</f>
+        <v>44827</v>
+      </c>
+      <c r="G15" s="8">
+        <v>0.375</v>
+      </c>
+      <c r="H15" s="8">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>1</v>
+      </c>
+      <c r="B16" s="6" t="str">
+        <f>TEXT(F16,"DD/MM/YYYY") &amp; " " &amp; TEXT(G16,"H:MM")</f>
+        <v>24/09/2022 9:00</v>
+      </c>
+      <c r="C16" s="1" t="str">
+        <f>TEXT(F16,"DD/MM/YYYY") &amp; " " &amp; TEXT(H16,"H:MM")</f>
+        <v>24/09/2022 15:00</v>
+      </c>
+      <c r="F16" s="7">
+        <f t="shared" ref="F16:F21" si="2">F15+1</f>
+        <v>44828</v>
+      </c>
+      <c r="G16" s="8">
+        <v>0.375</v>
+      </c>
+      <c r="H16" s="8">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>1</v>
+      </c>
+      <c r="B17" s="6" t="str">
+        <f>TEXT(F17,"DD/MM/YYYY") &amp; " " &amp; TEXT(G17,"H:MM")</f>
+        <v>25/09/2022 9:00</v>
+      </c>
+      <c r="C17" s="1" t="str">
+        <f>TEXT(F17,"DD/MM/YYYY") &amp; " " &amp; TEXT(H17,"H:MM")</f>
+        <v>25/09/2022 15:00</v>
+      </c>
+      <c r="F17" s="7">
+        <f t="shared" si="2"/>
+        <v>44829</v>
+      </c>
+      <c r="G17" s="8">
+        <v>0.375</v>
+      </c>
+      <c r="H17" s="8">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>1</v>
+      </c>
+      <c r="B18" s="6" t="str">
+        <f>TEXT(F18,"DD/MM/YYYY") &amp; " " &amp; TEXT(G18,"H:MM")</f>
+        <v>29/09/2022 9:00</v>
+      </c>
+      <c r="C18" s="1" t="str">
+        <f>TEXT(F18,"DD/MM/YYYY") &amp; " " &amp; TEXT(H18,"H:MM")</f>
+        <v>29/09/2022 15:00</v>
+      </c>
+      <c r="F18" s="7">
+        <f>F14+7</f>
+        <v>44833</v>
+      </c>
+      <c r="G18" s="8">
+        <v>0.375</v>
+      </c>
+      <c r="H18" s="8">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>1</v>
+      </c>
+      <c r="B19" s="6" t="str">
+        <f>TEXT(F19,"DD/MM/YYYY") &amp; " " &amp; TEXT(G19,"H:MM")</f>
+        <v>30/09/2022 9:00</v>
+      </c>
+      <c r="C19" s="1" t="str">
+        <f>TEXT(F19,"DD/MM/YYYY") &amp; " " &amp; TEXT(H19,"H:MM")</f>
+        <v>30/09/2022 15:00</v>
+      </c>
+      <c r="F19" s="7">
+        <f>F18+1</f>
+        <v>44834</v>
+      </c>
+      <c r="G19" s="8">
+        <v>0.375</v>
+      </c>
+      <c r="H19" s="8">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>1</v>
+      </c>
+      <c r="B20" s="6" t="str">
+        <f>TEXT(F20,"DD/MM/YYYY") &amp; " " &amp; TEXT(G20,"H:MM")</f>
+        <v>01/10/2022 9:00</v>
+      </c>
+      <c r="C20" s="1" t="str">
+        <f>TEXT(F20,"DD/MM/YYYY") &amp; " " &amp; TEXT(H20,"H:MM")</f>
+        <v>01/10/2022 15:00</v>
+      </c>
+      <c r="F20" s="7">
+        <f t="shared" ref="F20:F21" si="3">F19+1</f>
+        <v>44835</v>
+      </c>
+      <c r="G20" s="8">
+        <v>0.375</v>
+      </c>
+      <c r="H20" s="8">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>1</v>
+      </c>
+      <c r="B21" s="6" t="str">
+        <f>TEXT(F21,"DD/MM/YYYY") &amp; " " &amp; TEXT(G21,"H:MM")</f>
+        <v>02/10/2022 9:00</v>
+      </c>
+      <c r="C21" s="1" t="str">
+        <f>TEXT(F21,"DD/MM/YYYY") &amp; " " &amp; TEXT(H21,"H:MM")</f>
+        <v>02/10/2022 15:00</v>
+      </c>
+      <c r="F21" s="7">
+        <f t="shared" si="3"/>
+        <v>44836</v>
+      </c>
+      <c r="G21" s="8">
+        <v>0.375</v>
+      </c>
+      <c r="H21" s="8">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22" s="5" t="str">
+        <f>TEXT(F22,"DD/MM/YYYY") &amp; " " &amp; TEXT(G22,"H:MM")</f>
+        <v>03/09/2022 8:00</v>
+      </c>
+      <c r="C22" t="str">
+        <f>TEXT(F22,"DD/MM/YYYY") &amp; " " &amp; TEXT(H22,"H:MM")</f>
+        <v>03/09/2022 13:30</v>
+      </c>
+      <c r="E22" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="4">
         <v>44807</v>
       </c>
-      <c r="F4" s="3">
-        <v>0.375</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>1</v>
-      </c>
-      <c r="B5" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>04/09/2022 9:00</v>
-      </c>
-      <c r="C5" t="str">
-        <f t="shared" si="1"/>
-        <v>04/09/2022 15:00</v>
-      </c>
-      <c r="E5" s="4">
+      <c r="G22" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H22" s="3">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" s="5" t="str">
+        <f>TEXT(F23,"DD/MM/YYYY") &amp; " " &amp; TEXT(G23,"H:MM")</f>
+        <v>04/09/2022 8:00</v>
+      </c>
+      <c r="C23" t="str">
+        <f>TEXT(F23,"DD/MM/YYYY") &amp; " " &amp; TEXT(H23,"H:MM")</f>
+        <v>04/09/2022 13:30</v>
+      </c>
+      <c r="F23" s="4">
+        <f>F22+1</f>
         <v>44808</v>
       </c>
-      <c r="F5" s="3">
-        <v>0.375</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>1</v>
-      </c>
-      <c r="B6" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>08/09/2022 9:00</v>
-      </c>
-      <c r="C6" t="str">
-        <f t="shared" si="1"/>
-        <v>08/09/2022 15:00</v>
-      </c>
-      <c r="E6" s="4">
-        <f>E2+7</f>
-        <v>44812</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0.375</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>1</v>
-      </c>
-      <c r="B7" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>09/09/2022 9:00</v>
-      </c>
-      <c r="C7" t="str">
-        <f t="shared" si="1"/>
-        <v>09/09/2022 15:00</v>
-      </c>
-      <c r="E7" s="4">
-        <f>E6+1</f>
-        <v>44813</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0.375</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>1</v>
-      </c>
-      <c r="B8" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>10/09/2022 9:00</v>
-      </c>
-      <c r="C8" t="str">
-        <f t="shared" si="1"/>
-        <v>10/09/2022 15:00</v>
-      </c>
-      <c r="E8" s="4">
-        <f t="shared" ref="E8:E17" si="2">E7+1</f>
+      <c r="G23" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H23" s="3">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24" s="5" t="str">
+        <f>TEXT(F24,"DD/MM/YYYY") &amp; " " &amp; TEXT(G24,"H:MM")</f>
+        <v>10/09/2022 8:00</v>
+      </c>
+      <c r="C24" t="str">
+        <f>TEXT(F24,"DD/MM/YYYY") &amp; " " &amp; TEXT(H24,"H:MM")</f>
+        <v>10/09/2022 13:30</v>
+      </c>
+      <c r="F24" s="4">
+        <f>F22+7</f>
         <v>44814</v>
       </c>
-      <c r="F8" s="3">
-        <v>0.375</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>1</v>
-      </c>
-      <c r="B9" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>11/09/2022 9:00</v>
-      </c>
-      <c r="C9" t="str">
-        <f t="shared" si="1"/>
-        <v>11/09/2022 15:00</v>
-      </c>
-      <c r="E9" s="4">
-        <f t="shared" si="2"/>
+      <c r="G24" s="3">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="H24" s="3">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25" s="5" t="str">
+        <f>TEXT(F25,"DD/MM/YYYY") &amp; " " &amp; TEXT(G25,"H:MM")</f>
+        <v>11/09/2022 8:00</v>
+      </c>
+      <c r="C25" t="str">
+        <f>TEXT(F25,"DD/MM/YYYY") &amp; " " &amp; TEXT(H25,"H:MM")</f>
+        <v>11/09/2022 13:30</v>
+      </c>
+      <c r="F25" s="4">
+        <f>F24+1</f>
         <v>44815</v>
       </c>
-      <c r="F9" s="3">
-        <v>0.375</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>1</v>
-      </c>
-      <c r="B10" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>15/09/2022 9:00</v>
-      </c>
-      <c r="C10" t="str">
-        <f t="shared" si="1"/>
-        <v>15/09/2022 15:00</v>
-      </c>
-      <c r="E10" s="4">
-        <f>E6+7</f>
-        <v>44819</v>
-      </c>
-      <c r="F10" s="3">
-        <v>0.375</v>
-      </c>
-      <c r="G10" s="3">
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>1</v>
-      </c>
-      <c r="B11" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>16/09/2022 9:00</v>
-      </c>
-      <c r="C11" t="str">
-        <f t="shared" si="1"/>
-        <v>16/09/2022 15:00</v>
-      </c>
-      <c r="E11" s="4">
-        <f>E10+1</f>
-        <v>44820</v>
-      </c>
-      <c r="F11" s="3">
-        <v>0.375</v>
-      </c>
-      <c r="G11" s="3">
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>1</v>
-      </c>
-      <c r="B12" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>17/09/2022 9:00</v>
-      </c>
-      <c r="C12" t="str">
-        <f t="shared" si="1"/>
-        <v>17/09/2022 15:00</v>
-      </c>
-      <c r="E12" s="4">
-        <f t="shared" ref="E12:E21" si="3">E11+1</f>
+      <c r="G25" s="3">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="H25" s="3">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26" s="5" t="str">
+        <f>TEXT(F26,"DD/MM/YYYY") &amp; " " &amp; TEXT(G26,"H:MM")</f>
+        <v>17/09/2022 8:00</v>
+      </c>
+      <c r="C26" t="str">
+        <f>TEXT(F26,"DD/MM/YYYY") &amp; " " &amp; TEXT(H26,"H:MM")</f>
+        <v>17/09/2022 13:30</v>
+      </c>
+      <c r="F26" s="4">
+        <f>F24+7</f>
         <v>44821</v>
       </c>
-      <c r="F12" s="3">
-        <v>0.375</v>
-      </c>
-      <c r="G12" s="3">
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>1</v>
-      </c>
-      <c r="B13" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>18/09/2022 9:00</v>
-      </c>
-      <c r="C13" t="str">
-        <f t="shared" si="1"/>
-        <v>18/09/2022 15:00</v>
-      </c>
-      <c r="E13" s="4">
-        <f t="shared" si="3"/>
+      <c r="G26" s="3">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="H26" s="3">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27" s="5" t="str">
+        <f>TEXT(F27,"DD/MM/YYYY") &amp; " " &amp; TEXT(G27,"H:MM")</f>
+        <v>18/09/2022 8:00</v>
+      </c>
+      <c r="C27" t="str">
+        <f>TEXT(F27,"DD/MM/YYYY") &amp; " " &amp; TEXT(H27,"H:MM")</f>
+        <v>18/09/2022 13:30</v>
+      </c>
+      <c r="F27" s="4">
+        <f>F26+1</f>
         <v>44822</v>
       </c>
-      <c r="F13" s="3">
-        <v>0.375</v>
-      </c>
-      <c r="G13" s="3">
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>1</v>
-      </c>
-      <c r="B14" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>22/09/2022 9:00</v>
-      </c>
-      <c r="C14" t="str">
-        <f t="shared" si="1"/>
-        <v>22/09/2022 15:00</v>
-      </c>
-      <c r="E14" s="4">
-        <f>E10+7</f>
-        <v>44826</v>
-      </c>
-      <c r="F14" s="3">
-        <v>0.375</v>
-      </c>
-      <c r="G14" s="3">
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>1</v>
-      </c>
-      <c r="B15" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>23/09/2022 9:00</v>
-      </c>
-      <c r="C15" t="str">
-        <f t="shared" si="1"/>
-        <v>23/09/2022 15:00</v>
-      </c>
-      <c r="E15" s="4">
-        <f>E14+1</f>
-        <v>44827</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0.375</v>
-      </c>
-      <c r="G15" s="3">
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>1</v>
-      </c>
-      <c r="B16" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>24/09/2022 9:00</v>
-      </c>
-      <c r="C16" t="str">
-        <f t="shared" si="1"/>
-        <v>24/09/2022 15:00</v>
-      </c>
-      <c r="E16" s="4">
-        <f t="shared" ref="E16:E21" si="4">E15+1</f>
+      <c r="G27" s="3">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="H27" s="3">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="B28" s="5" t="str">
+        <f>TEXT(F28,"DD/MM/YYYY") &amp; " " &amp; TEXT(G28,"H:MM")</f>
+        <v>24/09/2022 8:00</v>
+      </c>
+      <c r="C28" t="str">
+        <f>TEXT(F28,"DD/MM/YYYY") &amp; " " &amp; TEXT(H28,"H:MM")</f>
+        <v>24/09/2022 13:30</v>
+      </c>
+      <c r="F28" s="4">
+        <f>F26+7</f>
         <v>44828</v>
       </c>
-      <c r="F16" s="3">
-        <v>0.375</v>
-      </c>
-      <c r="G16" s="3">
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>1</v>
-      </c>
-      <c r="B17" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>25/09/2022 9:00</v>
-      </c>
-      <c r="C17" t="str">
-        <f t="shared" si="1"/>
-        <v>25/09/2022 15:00</v>
-      </c>
-      <c r="E17" s="4">
-        <f t="shared" si="4"/>
+      <c r="G28" s="3">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="H28" s="3">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29" s="5" t="str">
+        <f>TEXT(F29,"DD/MM/YYYY") &amp; " " &amp; TEXT(G29,"H:MM")</f>
+        <v>25/09/2022 8:00</v>
+      </c>
+      <c r="C29" t="str">
+        <f>TEXT(F29,"DD/MM/YYYY") &amp; " " &amp; TEXT(H29,"H:MM")</f>
+        <v>25/09/2022 13:30</v>
+      </c>
+      <c r="F29" s="4">
+        <f>F28+1</f>
         <v>44829</v>
       </c>
-      <c r="F17" s="3">
-        <v>0.375</v>
-      </c>
-      <c r="G17" s="3">
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>1</v>
-      </c>
-      <c r="B18" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>29/09/2022 9:00</v>
-      </c>
-      <c r="C18" t="str">
-        <f t="shared" si="1"/>
-        <v>29/09/2022 15:00</v>
-      </c>
-      <c r="E18" s="4">
-        <f>E14+7</f>
-        <v>44833</v>
-      </c>
-      <c r="F18" s="3">
-        <v>0.375</v>
-      </c>
-      <c r="G18" s="3">
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>1</v>
-      </c>
-      <c r="B19" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>30/09/2022 9:00</v>
-      </c>
-      <c r="C19" t="str">
-        <f t="shared" si="1"/>
-        <v>30/09/2022 15:00</v>
-      </c>
-      <c r="E19" s="4">
-        <f>E18+1</f>
-        <v>44834</v>
-      </c>
-      <c r="F19" s="3">
-        <v>0.375</v>
-      </c>
-      <c r="G19" s="3">
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
-        <v>1</v>
-      </c>
-      <c r="B20" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>01/10/2022 9:00</v>
-      </c>
-      <c r="C20" t="str">
-        <f t="shared" si="1"/>
-        <v>01/10/2022 15:00</v>
-      </c>
-      <c r="E20" s="4">
-        <f t="shared" ref="E20:E21" si="5">E19+1</f>
+      <c r="G29" s="3">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="H29" s="3">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30" s="5" t="str">
+        <f>TEXT(F30,"DD/MM/YYYY") &amp; " " &amp; TEXT(G30,"H:MM")</f>
+        <v>01/10/2022 8:00</v>
+      </c>
+      <c r="C30" t="str">
+        <f>TEXT(F30,"DD/MM/YYYY") &amp; " " &amp; TEXT(H30,"H:MM")</f>
+        <v>01/10/2022 13:30</v>
+      </c>
+      <c r="F30" s="4">
+        <f>F28+7</f>
         <v>44835</v>
       </c>
-      <c r="F20" s="3">
-        <v>0.375</v>
-      </c>
-      <c r="G20" s="3">
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>1</v>
-      </c>
-      <c r="B21" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>02/10/2022 9:00</v>
-      </c>
-      <c r="C21" t="str">
-        <f t="shared" si="1"/>
-        <v>02/10/2022 15:00</v>
-      </c>
-      <c r="E21" s="4">
-        <f t="shared" si="5"/>
+      <c r="G30" s="3">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="H30" s="3">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31" s="5" t="str">
+        <f>TEXT(F31,"DD/MM/YYYY") &amp; " " &amp; TEXT(G31,"H:MM")</f>
+        <v>02/10/2022 8:00</v>
+      </c>
+      <c r="C31" t="str">
+        <f>TEXT(F31,"DD/MM/YYYY") &amp; " " &amp; TEXT(H31,"H:MM")</f>
+        <v>02/10/2022 13:30</v>
+      </c>
+      <c r="F31" s="4">
+        <f>F30+1</f>
         <v>44836</v>
       </c>
-      <c r="F21" s="3">
-        <v>0.375</v>
-      </c>
-      <c r="G21" s="3">
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>2</v>
-      </c>
-      <c r="B22" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>01/09/2022 8:00</v>
-      </c>
-      <c r="C22" t="str">
-        <f t="shared" si="1"/>
-        <v>01/09/2022 13:30</v>
-      </c>
-      <c r="E22" s="4">
-        <v>44805</v>
-      </c>
-      <c r="F22" s="3">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="G22" s="3">
+      <c r="G31" s="3">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="H31" s="3">
         <v>0.5625</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>2</v>
-      </c>
-      <c r="B23" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>02/09/2022 8:00</v>
-      </c>
-      <c r="C23" t="str">
-        <f t="shared" si="1"/>
-        <v>02/09/2022 13:30</v>
-      </c>
-      <c r="E23" s="4">
-        <v>44806</v>
-      </c>
-      <c r="F23" s="3">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="G23" s="3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>2</v>
+      </c>
+      <c r="B32" s="5" t="str">
+        <f>TEXT(F32,"DD/MM/YYYY") &amp; " " &amp; TEXT(G32,"H:MM")</f>
+        <v>08/10/2022 8:00</v>
+      </c>
+      <c r="C32" t="str">
+        <f>TEXT(F32,"DD/MM/YYYY") &amp; " " &amp; TEXT(H32,"H:MM")</f>
+        <v>08/10/2022 13:30</v>
+      </c>
+      <c r="F32" s="4">
+        <f>F30+7</f>
+        <v>44842</v>
+      </c>
+      <c r="G32" s="3">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="H32" s="3">
         <v>0.5625</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>2</v>
-      </c>
-      <c r="B24" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>03/09/2022 8:00</v>
-      </c>
-      <c r="C24" t="str">
-        <f t="shared" si="1"/>
-        <v>03/09/2022 13:30</v>
-      </c>
-      <c r="E24" s="4">
-        <v>44807</v>
-      </c>
-      <c r="F24" s="3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>2</v>
+      </c>
+      <c r="B33" s="5" t="str">
+        <f>TEXT(F33,"DD/MM/YYYY") &amp; " " &amp; TEXT(G33,"H:MM")</f>
+        <v>09/10/2022 8:00</v>
+      </c>
+      <c r="C33" t="str">
+        <f>TEXT(F33,"DD/MM/YYYY") &amp; " " &amp; TEXT(H33,"H:MM")</f>
+        <v>09/10/2022 13:30</v>
+      </c>
+      <c r="F33" s="4">
+        <f>F32+1</f>
+        <v>44843</v>
+      </c>
+      <c r="G33" s="3">
         <v>0.33333333333333298</v>
       </c>
-      <c r="G24" s="3">
+      <c r="H33" s="3">
         <v>0.5625</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>2</v>
-      </c>
-      <c r="B25" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>04/09/2022 8:00</v>
-      </c>
-      <c r="C25" t="str">
-        <f t="shared" si="1"/>
-        <v>04/09/2022 13:30</v>
-      </c>
-      <c r="E25" s="4">
-        <v>44808</v>
-      </c>
-      <c r="F25" s="3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34" s="5" t="str">
+        <f>TEXT(F34,"DD/MM/YYYY") &amp; " " &amp; TEXT(G34,"H:MM")</f>
+        <v>15/10/2022 8:00</v>
+      </c>
+      <c r="C34" t="str">
+        <f>TEXT(F34,"DD/MM/YYYY") &amp; " " &amp; TEXT(H34,"H:MM")</f>
+        <v>15/10/2022 13:30</v>
+      </c>
+      <c r="F34" s="4">
+        <f>F32+7</f>
+        <v>44849</v>
+      </c>
+      <c r="G34" s="3">
         <v>0.33333333333333298</v>
       </c>
-      <c r="G25" s="3">
+      <c r="H34" s="3">
         <v>0.5625</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>2</v>
-      </c>
-      <c r="B26" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>08/09/2022 8:00</v>
-      </c>
-      <c r="C26" t="str">
-        <f t="shared" si="1"/>
-        <v>08/09/2022 13:30</v>
-      </c>
-      <c r="E26" s="4">
-        <f>E22+7</f>
-        <v>44812</v>
-      </c>
-      <c r="F26" s="3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>3</v>
+      </c>
+      <c r="B35" s="5" t="str">
+        <f>TEXT(F35,"DD/MM/YYYY") &amp; " " &amp; TEXT(G35,"H:MM")</f>
+        <v>16/10/2022 8:00</v>
+      </c>
+      <c r="C35" t="str">
+        <f>TEXT(F35,"DD/MM/YYYY") &amp; " " &amp; TEXT(H35,"H:MM")</f>
+        <v>16/10/2022 13:30</v>
+      </c>
+      <c r="F35" s="4">
+        <f>F34+1</f>
+        <v>44850</v>
+      </c>
+      <c r="G35" s="3">
         <v>0.33333333333333298</v>
       </c>
-      <c r="G26" s="3">
+      <c r="H35" s="3">
         <v>0.5625</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>2</v>
-      </c>
-      <c r="B27" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>09/09/2022 8:00</v>
-      </c>
-      <c r="C27" t="str">
-        <f t="shared" si="1"/>
-        <v>09/09/2022 13:30</v>
-      </c>
-      <c r="E27" s="4">
-        <f>E26+1</f>
-        <v>44813</v>
-      </c>
-      <c r="F27" s="3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>3</v>
+      </c>
+      <c r="B36" s="5" t="str">
+        <f>TEXT(F36,"DD/MM/YYYY") &amp; " " &amp; TEXT(G36,"H:MM")</f>
+        <v>22/10/2022 8:00</v>
+      </c>
+      <c r="C36" t="str">
+        <f>TEXT(F36,"DD/MM/YYYY") &amp; " " &amp; TEXT(H36,"H:MM")</f>
+        <v>22/10/2022 13:30</v>
+      </c>
+      <c r="F36" s="4">
+        <f>F34+7</f>
+        <v>44856</v>
+      </c>
+      <c r="G36" s="3">
         <v>0.33333333333333298</v>
       </c>
-      <c r="G27" s="3">
+      <c r="H36" s="3">
         <v>0.5625</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>2</v>
-      </c>
-      <c r="B28" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>10/09/2022 8:00</v>
-      </c>
-      <c r="C28" t="str">
-        <f t="shared" si="1"/>
-        <v>10/09/2022 13:30</v>
-      </c>
-      <c r="E28" s="4">
-        <f t="shared" ref="E28:E37" si="6">E27+1</f>
-        <v>44814</v>
-      </c>
-      <c r="F28" s="3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>3</v>
+      </c>
+      <c r="B37" s="5" t="str">
+        <f>TEXT(F37,"DD/MM/YYYY") &amp; " " &amp; TEXT(G37,"H:MM")</f>
+        <v>23/10/2022 8:00</v>
+      </c>
+      <c r="C37" t="str">
+        <f>TEXT(F37,"DD/MM/YYYY") &amp; " " &amp; TEXT(H37,"H:MM")</f>
+        <v>23/10/2022 13:30</v>
+      </c>
+      <c r="F37" s="4">
+        <f>F36+1</f>
+        <v>44857</v>
+      </c>
+      <c r="G37" s="3">
         <v>0.33333333333333298</v>
       </c>
-      <c r="G28" s="3">
+      <c r="H37" s="3">
         <v>0.5625</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>2</v>
-      </c>
-      <c r="B29" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>11/09/2022 8:00</v>
-      </c>
-      <c r="C29" t="str">
-        <f t="shared" si="1"/>
-        <v>11/09/2022 13:30</v>
-      </c>
-      <c r="E29" s="4">
-        <f t="shared" si="6"/>
-        <v>44815</v>
-      </c>
-      <c r="F29" s="3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>3</v>
+      </c>
+      <c r="B38" s="5" t="str">
+        <f>TEXT(F38,"DD/MM/YYYY") &amp; " " &amp; TEXT(G38,"H:MM")</f>
+        <v>29/10/2022 8:00</v>
+      </c>
+      <c r="C38" t="str">
+        <f>TEXT(F38,"DD/MM/YYYY") &amp; " " &amp; TEXT(H38,"H:MM")</f>
+        <v>29/10/2022 13:30</v>
+      </c>
+      <c r="F38" s="4">
+        <f>F36+7</f>
+        <v>44863</v>
+      </c>
+      <c r="G38" s="3">
         <v>0.33333333333333298</v>
       </c>
-      <c r="G29" s="3">
+      <c r="H38" s="3">
         <v>0.5625</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>2</v>
-      </c>
-      <c r="B30" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>15/09/2022 8:00</v>
-      </c>
-      <c r="C30" t="str">
-        <f t="shared" si="1"/>
-        <v>15/09/2022 13:30</v>
-      </c>
-      <c r="E30" s="4">
-        <f>E26+7</f>
-        <v>44819</v>
-      </c>
-      <c r="F30" s="3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>3</v>
+      </c>
+      <c r="B39" s="5" t="str">
+        <f>TEXT(F39,"DD/MM/YYYY") &amp; " " &amp; TEXT(G39,"H:MM")</f>
+        <v>30/10/2022 8:00</v>
+      </c>
+      <c r="C39" t="str">
+        <f>TEXT(F39,"DD/MM/YYYY") &amp; " " &amp; TEXT(H39,"H:MM")</f>
+        <v>30/10/2022 13:30</v>
+      </c>
+      <c r="F39" s="4">
+        <f>F38+1</f>
+        <v>44864</v>
+      </c>
+      <c r="G39" s="3">
         <v>0.33333333333333298</v>
       </c>
-      <c r="G30" s="3">
+      <c r="H39" s="3">
         <v>0.5625</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>2</v>
-      </c>
-      <c r="B31" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>16/09/2022 8:00</v>
-      </c>
-      <c r="C31" t="str">
-        <f t="shared" si="1"/>
-        <v>16/09/2022 13:30</v>
-      </c>
-      <c r="E31" s="4">
-        <f>E30+1</f>
-        <v>44820</v>
-      </c>
-      <c r="F31" s="3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>3</v>
+      </c>
+      <c r="B40" s="5" t="str">
+        <f>TEXT(F40,"DD/MM/YYYY") &amp; " " &amp; TEXT(G40,"H:MM")</f>
+        <v>05/11/2022 8:00</v>
+      </c>
+      <c r="C40" t="str">
+        <f>TEXT(F40,"DD/MM/YYYY") &amp; " " &amp; TEXT(H40,"H:MM")</f>
+        <v>05/11/2022 13:30</v>
+      </c>
+      <c r="F40" s="4">
+        <f>F38+7</f>
+        <v>44870</v>
+      </c>
+      <c r="G40" s="3">
         <v>0.33333333333333298</v>
       </c>
-      <c r="G31" s="3">
+      <c r="H40" s="3">
         <v>0.5625</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>2</v>
-      </c>
-      <c r="B32" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>17/09/2022 8:00</v>
-      </c>
-      <c r="C32" t="str">
-        <f t="shared" si="1"/>
-        <v>17/09/2022 13:30</v>
-      </c>
-      <c r="E32" s="4">
-        <f t="shared" ref="E32:E41" si="7">E31+1</f>
-        <v>44821</v>
-      </c>
-      <c r="F32" s="3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>3</v>
+      </c>
+      <c r="B41" s="5" t="str">
+        <f>TEXT(F41,"DD/MM/YYYY") &amp; " " &amp; TEXT(G41,"H:MM")</f>
+        <v>06/11/2022 8:00</v>
+      </c>
+      <c r="C41" t="str">
+        <f>TEXT(F41,"DD/MM/YYYY") &amp; " " &amp; TEXT(H41,"H:MM")</f>
+        <v>06/11/2022 13:30</v>
+      </c>
+      <c r="F41" s="4">
+        <f>F40+1</f>
+        <v>44871</v>
+      </c>
+      <c r="G41" s="3">
         <v>0.33333333333333298</v>
       </c>
-      <c r="G32" s="3">
+      <c r="H41" s="3">
         <v>0.5625</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>2</v>
-      </c>
-      <c r="B33" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>18/09/2022 8:00</v>
-      </c>
-      <c r="C33" t="str">
-        <f t="shared" si="1"/>
-        <v>18/09/2022 13:30</v>
-      </c>
-      <c r="E33" s="4">
-        <f t="shared" si="7"/>
-        <v>44822</v>
-      </c>
-      <c r="F33" s="3">
-        <v>0.33333333333333298</v>
-      </c>
-      <c r="G33" s="3">
-        <v>0.5625</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>2</v>
-      </c>
-      <c r="B34" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>22/09/2022 8:00</v>
-      </c>
-      <c r="C34" t="str">
-        <f t="shared" si="1"/>
-        <v>22/09/2022 13:30</v>
-      </c>
-      <c r="E34" s="4">
-        <f>E30+7</f>
-        <v>44826</v>
-      </c>
-      <c r="F34" s="3">
-        <v>0.33333333333333298</v>
-      </c>
-      <c r="G34" s="3">
-        <v>0.5625</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>2</v>
-      </c>
-      <c r="B35" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>23/09/2022 8:00</v>
-      </c>
-      <c r="C35" t="str">
-        <f t="shared" si="1"/>
-        <v>23/09/2022 13:30</v>
-      </c>
-      <c r="E35" s="4">
-        <f>E34+1</f>
-        <v>44827</v>
-      </c>
-      <c r="F35" s="3">
-        <v>0.33333333333333298</v>
-      </c>
-      <c r="G35" s="3">
-        <v>0.5625</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>2</v>
-      </c>
-      <c r="B36" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>24/09/2022 8:00</v>
-      </c>
-      <c r="C36" t="str">
-        <f t="shared" si="1"/>
-        <v>24/09/2022 13:30</v>
-      </c>
-      <c r="E36" s="4">
-        <f t="shared" ref="E36:E41" si="8">E35+1</f>
-        <v>44828</v>
-      </c>
-      <c r="F36" s="3">
-        <v>0.33333333333333298</v>
-      </c>
-      <c r="G36" s="3">
-        <v>0.5625</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>2</v>
-      </c>
-      <c r="B37" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>25/09/2022 8:00</v>
-      </c>
-      <c r="C37" t="str">
-        <f t="shared" si="1"/>
-        <v>25/09/2022 13:30</v>
-      </c>
-      <c r="E37" s="4">
-        <f t="shared" si="8"/>
-        <v>44829</v>
-      </c>
-      <c r="F37" s="3">
-        <v>0.33333333333333298</v>
-      </c>
-      <c r="G37" s="3">
-        <v>0.5625</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>2</v>
-      </c>
-      <c r="B38" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>29/09/2022 8:00</v>
-      </c>
-      <c r="C38" t="str">
-        <f t="shared" si="1"/>
-        <v>29/09/2022 13:30</v>
-      </c>
-      <c r="E38" s="4">
-        <f>E34+7</f>
-        <v>44833</v>
-      </c>
-      <c r="F38" s="3">
-        <v>0.33333333333333298</v>
-      </c>
-      <c r="G38" s="3">
-        <v>0.5625</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>2</v>
-      </c>
-      <c r="B39" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>30/09/2022 8:00</v>
-      </c>
-      <c r="C39" t="str">
-        <f t="shared" si="1"/>
-        <v>30/09/2022 13:30</v>
-      </c>
-      <c r="E39" s="4">
-        <f>E38+1</f>
-        <v>44834</v>
-      </c>
-      <c r="F39" s="3">
-        <v>0.33333333333333298</v>
-      </c>
-      <c r="G39" s="3">
-        <v>0.5625</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>2</v>
-      </c>
-      <c r="B40" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>01/10/2022 8:00</v>
-      </c>
-      <c r="C40" t="str">
-        <f t="shared" si="1"/>
-        <v>01/10/2022 13:30</v>
-      </c>
-      <c r="E40" s="4">
-        <f t="shared" ref="E40:E41" si="9">E39+1</f>
-        <v>44835</v>
-      </c>
-      <c r="F40" s="3">
-        <v>0.33333333333333298</v>
-      </c>
-      <c r="G40" s="3">
-        <v>0.5625</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>2</v>
-      </c>
-      <c r="B41" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>02/10/2022 8:00</v>
-      </c>
-      <c r="C41" t="str">
-        <f t="shared" si="1"/>
-        <v>02/10/2022 13:30</v>
-      </c>
-      <c r="E41" s="4">
-        <f t="shared" si="9"/>
+    <row r="42" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>3</v>
+      </c>
+      <c r="B42" s="6" t="str">
+        <f>TEXT(F42,"DD/MM/YYYY") &amp; " " &amp; TEXT(G42,"H:MM")</f>
+        <v>02/10/2022 7:30</v>
+      </c>
+      <c r="C42" s="1" t="str">
+        <f>TEXT(F42,"DD/MM/YYYY") &amp; " " &amp; TEXT(H42,"H:MM")</f>
+        <v>02/10/2022 14:00</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F42" s="7">
+        <f>F30+1</f>
         <v>44836</v>
       </c>
-      <c r="F41" s="3">
-        <v>0.33333333333333298</v>
-      </c>
-      <c r="G41" s="3">
-        <v>0.5625</v>
+      <c r="G42" s="8">
+        <v>0.3125</v>
+      </c>
+      <c r="H42" s="8">
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>3</v>
+      </c>
+      <c r="B43" s="6" t="str">
+        <f>TEXT(F43,"DD/MM/YYYY") &amp; " " &amp; TEXT(G43,"H:MM")</f>
+        <v>30/10/2022 7:30</v>
+      </c>
+      <c r="C43" s="1" t="str">
+        <f>TEXT(F43,"DD/MM/YYYY") &amp; " " &amp; TEXT(H43,"H:MM")</f>
+        <v>30/10/2022 14:00</v>
+      </c>
+      <c r="F43" s="7">
+        <f>F42+28</f>
+        <v>44864</v>
+      </c>
+      <c r="G43" s="8">
+        <v>0.3125</v>
+      </c>
+      <c r="H43" s="8">
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>3</v>
+      </c>
+      <c r="B44" s="6" t="str">
+        <f>TEXT(F44,"DD/MM/YYYY") &amp; " " &amp; TEXT(G44,"H:MM")</f>
+        <v>04/12/2022 7:30</v>
+      </c>
+      <c r="C44" s="1" t="str">
+        <f>TEXT(F44,"DD/MM/YYYY") &amp; " " &amp; TEXT(H44,"H:MM")</f>
+        <v>04/12/2022 14:00</v>
+      </c>
+      <c r="F44" s="7">
+        <f>F43+35</f>
+        <v>44899</v>
+      </c>
+      <c r="G44" s="8">
+        <v>0.3125</v>
+      </c>
+      <c r="H44" s="8">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>3</v>
+      </c>
+      <c r="B45" s="6" t="str">
+        <f>TEXT(F45,"DD/MM/YYYY") &amp; " " &amp; TEXT(G45,"H:MM")</f>
+        <v>01/01/2023 7:30</v>
+      </c>
+      <c r="C45" s="1" t="str">
+        <f>TEXT(F45,"DD/MM/YYYY") &amp; " " &amp; TEXT(H45,"H:MM")</f>
+        <v>01/01/2023 14:00</v>
+      </c>
+      <c r="F45" s="7">
+        <f t="shared" ref="F45:F46" si="4">F44+28</f>
+        <v>44927</v>
+      </c>
+      <c r="G45" s="8">
+        <v>0.3125</v>
+      </c>
+      <c r="H45" s="8">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>3</v>
+      </c>
+      <c r="B46" s="6" t="str">
+        <f>TEXT(F46,"DD/MM/YYYY") &amp; " " &amp; TEXT(G46,"H:MM")</f>
+        <v>05/02/2023 7:30</v>
+      </c>
+      <c r="C46" s="1" t="str">
+        <f>TEXT(F46,"DD/MM/YYYY") &amp; " " &amp; TEXT(H46,"H:MM")</f>
+        <v>05/02/2023 14:00</v>
+      </c>
+      <c r="F46" s="7">
+        <f>F45+35</f>
+        <v>44962</v>
+      </c>
+      <c r="G46" s="8">
+        <v>0.3125</v>
+      </c>
+      <c r="H46" s="8">
+        <v>0.58333333333333304</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Have managed to seed events, booking and eventsbooking.
</commit_message>
<xml_diff>
--- a/seeds/Formulaic Seed generation.xlsx
+++ b/seeds/Formulaic Seed generation.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reeveschragger/Documents/Bootcamp/Projects/Farmers-Market-Organiser/seeds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0D6663-B6D6-C242-B615-A5AD156A5665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EEF60C2-1F52-5F48-9FA9-44BE27B77045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16340" activeTab="1" xr2:uid="{E72EE37F-B9BE-8B4C-AF7C-D3608E94063D}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16340" activeTab="2" xr2:uid="{E72EE37F-B9BE-8B4C-AF7C-D3608E94063D}"/>
   </bookViews>
   <sheets>
     <sheet name="Stall" sheetId="1" r:id="rId1"/>
     <sheet name="Event" sheetId="2" r:id="rId2"/>
+    <sheet name="Booking EventsBooking" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="170">
   <si>
     <t>stall_name</t>
   </si>
@@ -240,6 +241,312 @@
   </si>
   <si>
     <t>Eastern 3</t>
+  </si>
+  <si>
+    <t>Likely_Stall_ID</t>
+  </si>
+  <si>
+    <t>event_id</t>
+  </si>
+  <si>
+    <t>stall_id</t>
+  </si>
+  <si>
+    <t>lease_start</t>
+  </si>
+  <si>
+    <t>event_id(ikely)</t>
+  </si>
+  <si>
+    <t>3days</t>
+  </si>
+  <si>
+    <t>1 day</t>
+  </si>
+  <si>
+    <t>Booking</t>
+  </si>
+  <si>
+    <t>EventsBooking</t>
+  </si>
+  <si>
+    <t>booking_id</t>
+  </si>
+  <si>
+    <t>01/09/2022 9:00</t>
+  </si>
+  <si>
+    <t>01/09/2022 15:00</t>
+  </si>
+  <si>
+    <t>02/09/2022 9:00</t>
+  </si>
+  <si>
+    <t>02/09/2022 15:00</t>
+  </si>
+  <si>
+    <t>03/09/2022 9:00</t>
+  </si>
+  <si>
+    <t>03/09/2022 15:00</t>
+  </si>
+  <si>
+    <t>04/09/2022 9:00</t>
+  </si>
+  <si>
+    <t>04/09/2022 15:00</t>
+  </si>
+  <si>
+    <t>08/09/2022 9:00</t>
+  </si>
+  <si>
+    <t>08/09/2022 15:00</t>
+  </si>
+  <si>
+    <t>09/09/2022 9:00</t>
+  </si>
+  <si>
+    <t>09/09/2022 15:00</t>
+  </si>
+  <si>
+    <t>10/09/2022 9:00</t>
+  </si>
+  <si>
+    <t>10/09/2022 15:00</t>
+  </si>
+  <si>
+    <t>11/09/2022 9:00</t>
+  </si>
+  <si>
+    <t>11/09/2022 15:00</t>
+  </si>
+  <si>
+    <t>15/09/2022 9:00</t>
+  </si>
+  <si>
+    <t>15/09/2022 15:00</t>
+  </si>
+  <si>
+    <t>16/09/2022 9:00</t>
+  </si>
+  <si>
+    <t>16/09/2022 15:00</t>
+  </si>
+  <si>
+    <t>17/09/2022 9:00</t>
+  </si>
+  <si>
+    <t>17/09/2022 15:00</t>
+  </si>
+  <si>
+    <t>18/09/2022 9:00</t>
+  </si>
+  <si>
+    <t>18/09/2022 15:00</t>
+  </si>
+  <si>
+    <t>22/09/2022 9:00</t>
+  </si>
+  <si>
+    <t>22/09/2022 15:00</t>
+  </si>
+  <si>
+    <t>23/09/2022 9:00</t>
+  </si>
+  <si>
+    <t>23/09/2022 15:00</t>
+  </si>
+  <si>
+    <t>24/09/2022 9:00</t>
+  </si>
+  <si>
+    <t>24/09/2022 15:00</t>
+  </si>
+  <si>
+    <t>25/09/2022 9:00</t>
+  </si>
+  <si>
+    <t>25/09/2022 15:00</t>
+  </si>
+  <si>
+    <t>29/09/2022 9:00</t>
+  </si>
+  <si>
+    <t>29/09/2022 15:00</t>
+  </si>
+  <si>
+    <t>30/09/2022 9:00</t>
+  </si>
+  <si>
+    <t>30/09/2022 15:00</t>
+  </si>
+  <si>
+    <t>01/10/2022 9:00</t>
+  </si>
+  <si>
+    <t>01/10/2022 15:00</t>
+  </si>
+  <si>
+    <t>02/10/2022 9:00</t>
+  </si>
+  <si>
+    <t>02/10/2022 15:00</t>
+  </si>
+  <si>
+    <t>03/09/2022 8:00</t>
+  </si>
+  <si>
+    <t>03/09/2022 13:30</t>
+  </si>
+  <si>
+    <t>04/09/2022 8:00</t>
+  </si>
+  <si>
+    <t>04/09/2022 13:30</t>
+  </si>
+  <si>
+    <t>10/09/2022 8:00</t>
+  </si>
+  <si>
+    <t>10/09/2022 13:30</t>
+  </si>
+  <si>
+    <t>11/09/2022 8:00</t>
+  </si>
+  <si>
+    <t>11/09/2022 13:30</t>
+  </si>
+  <si>
+    <t>17/09/2022 8:00</t>
+  </si>
+  <si>
+    <t>17/09/2022 13:30</t>
+  </si>
+  <si>
+    <t>18/09/2022 8:00</t>
+  </si>
+  <si>
+    <t>18/09/2022 13:30</t>
+  </si>
+  <si>
+    <t>24/09/2022 8:00</t>
+  </si>
+  <si>
+    <t>24/09/2022 13:30</t>
+  </si>
+  <si>
+    <t>25/09/2022 8:00</t>
+  </si>
+  <si>
+    <t>25/09/2022 13:30</t>
+  </si>
+  <si>
+    <t>01/10/2022 8:00</t>
+  </si>
+  <si>
+    <t>01/10/2022 13:30</t>
+  </si>
+  <si>
+    <t>02/10/2022 8:00</t>
+  </si>
+  <si>
+    <t>02/10/2022 13:30</t>
+  </si>
+  <si>
+    <t>08/10/2022 8:00</t>
+  </si>
+  <si>
+    <t>08/10/2022 13:30</t>
+  </si>
+  <si>
+    <t>09/10/2022 8:00</t>
+  </si>
+  <si>
+    <t>09/10/2022 13:30</t>
+  </si>
+  <si>
+    <t>15/10/2022 8:00</t>
+  </si>
+  <si>
+    <t>15/10/2022 13:30</t>
+  </si>
+  <si>
+    <t>16/10/2022 8:00</t>
+  </si>
+  <si>
+    <t>16/10/2022 13:30</t>
+  </si>
+  <si>
+    <t>22/10/2022 8:00</t>
+  </si>
+  <si>
+    <t>22/10/2022 13:30</t>
+  </si>
+  <si>
+    <t>23/10/2022 8:00</t>
+  </si>
+  <si>
+    <t>23/10/2022 13:30</t>
+  </si>
+  <si>
+    <t>29/10/2022 8:00</t>
+  </si>
+  <si>
+    <t>29/10/2022 13:30</t>
+  </si>
+  <si>
+    <t>30/10/2022 8:00</t>
+  </si>
+  <si>
+    <t>30/10/2022 13:30</t>
+  </si>
+  <si>
+    <t>05/11/2022 8:00</t>
+  </si>
+  <si>
+    <t>05/11/2022 13:30</t>
+  </si>
+  <si>
+    <t>06/11/2022 8:00</t>
+  </si>
+  <si>
+    <t>06/11/2022 13:30</t>
+  </si>
+  <si>
+    <t>02/10/2022 7:30</t>
+  </si>
+  <si>
+    <t>02/10/2022 14:00</t>
+  </si>
+  <si>
+    <t>30/10/2022 7:30</t>
+  </si>
+  <si>
+    <t>30/10/2022 14:00</t>
+  </si>
+  <si>
+    <t>04/12/2022 7:30</t>
+  </si>
+  <si>
+    <t>04/12/2022 14:00</t>
+  </si>
+  <si>
+    <t>01/01/2023 7:30</t>
+  </si>
+  <si>
+    <t>01/01/2023 14:00</t>
+  </si>
+  <si>
+    <t>05/02/2023 7:30</t>
+  </si>
+  <si>
+    <t>05/02/2023 14:00</t>
+  </si>
+  <si>
+    <t>lease_expiry</t>
+  </si>
+  <si>
+    <t>stallholder_id</t>
   </si>
 </sst>
 </file>
@@ -247,8 +554,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="171" formatCode="[$-C09]dddd\,\ d/m/yyyy;@"/>
-    <numFmt numFmtId="172" formatCode="[$-409]h:mm:ss\ am/pm;@"/>
+    <numFmt numFmtId="164" formatCode="[$-C09]dddd\,\ d/m/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="[$-409]h:mm:ss\ AM/PM;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -271,7 +578,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -284,8 +591,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -293,20 +618,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -621,10 +970,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80609DE7-2449-714B-A221-516362804272}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D14" sqref="D1:D1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F58" sqref="A1:F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -632,7 +981,7 @@
     <col min="2" max="2" width="36.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -645,8 +994,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -659,8 +1011,11 @@
       <c r="D2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -673,8 +1028,12 @@
       <c r="D3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <f>F2+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -687,8 +1046,12 @@
       <c r="D4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <f t="shared" ref="F4:F58" si="0">F3+1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -701,8 +1064,12 @@
       <c r="D5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -715,8 +1082,12 @@
       <c r="D6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -729,8 +1100,12 @@
       <c r="D7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -743,8 +1118,12 @@
       <c r="D8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -757,8 +1136,12 @@
       <c r="D9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -771,8 +1154,12 @@
       <c r="D10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -785,8 +1172,12 @@
       <c r="D11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -799,8 +1190,12 @@
       <c r="D12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -813,8 +1208,12 @@
       <c r="D13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -827,8 +1226,12 @@
       <c r="D14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -841,8 +1244,12 @@
       <c r="D15" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -855,8 +1262,12 @@
       <c r="D16" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
@@ -869,8 +1280,12 @@
       <c r="D17" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>29</v>
       </c>
@@ -883,8 +1298,12 @@
       <c r="D18" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
@@ -897,8 +1316,12 @@
       <c r="D19" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
@@ -911,8 +1334,12 @@
       <c r="D20" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>32</v>
       </c>
@@ -925,8 +1352,12 @@
       <c r="D21" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>33</v>
       </c>
@@ -939,8 +1370,12 @@
       <c r="D22" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -953,8 +1388,12 @@
       <c r="D23">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -967,8 +1406,12 @@
       <c r="D24">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -981,8 +1424,12 @@
       <c r="D25">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -995,8 +1442,12 @@
       <c r="D26">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -1009,8 +1460,12 @@
       <c r="D27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -1023,8 +1478,12 @@
       <c r="D28">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -1037,8 +1496,12 @@
       <c r="D29">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -1051,8 +1514,12 @@
       <c r="D30">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -1065,8 +1532,12 @@
       <c r="D31">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -1079,8 +1550,12 @@
       <c r="D32">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -1093,8 +1568,12 @@
       <c r="D33">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>45</v>
       </c>
@@ -1107,8 +1586,12 @@
       <c r="D34">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>46</v>
       </c>
@@ -1121,8 +1604,12 @@
       <c r="D35">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>47</v>
       </c>
@@ -1135,8 +1622,12 @@
       <c r="D36">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>48</v>
       </c>
@@ -1149,8 +1640,12 @@
       <c r="D37">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>49</v>
       </c>
@@ -1163,8 +1658,12 @@
       <c r="D38">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>50</v>
       </c>
@@ -1177,8 +1676,12 @@
       <c r="D39">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>51</v>
       </c>
@@ -1191,8 +1694,12 @@
       <c r="D40">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F40">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -1205,8 +1712,12 @@
       <c r="D41">
         <v>2</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>53</v>
       </c>
@@ -1219,8 +1730,12 @@
       <c r="D42">
         <v>2</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>54</v>
       </c>
@@ -1232,6 +1747,280 @@
       </c>
       <c r="D43">
         <v>2</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" s="10">
+        <v>25</v>
+      </c>
+      <c r="D44">
+        <v>3</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45" s="10">
+        <v>25</v>
+      </c>
+      <c r="D45">
+        <v>3</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C46" s="10">
+        <v>25</v>
+      </c>
+      <c r="D46">
+        <v>3</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47" s="10">
+        <v>25</v>
+      </c>
+      <c r="D47">
+        <v>3</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C48" s="10">
+        <v>40</v>
+      </c>
+      <c r="D48">
+        <v>3</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C49" s="10">
+        <v>40</v>
+      </c>
+      <c r="D49">
+        <v>3</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50" s="10">
+        <v>40</v>
+      </c>
+      <c r="D50">
+        <v>3</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C51" s="10">
+        <v>40</v>
+      </c>
+      <c r="D51">
+        <v>3</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C52" s="10">
+        <v>40</v>
+      </c>
+      <c r="D52">
+        <v>3</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C53" s="10">
+        <v>40</v>
+      </c>
+      <c r="D53">
+        <v>3</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C54" s="10">
+        <v>45</v>
+      </c>
+      <c r="D54">
+        <v>3</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55" s="10">
+        <v>45</v>
+      </c>
+      <c r="D55">
+        <v>3</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C56" s="10">
+        <v>45</v>
+      </c>
+      <c r="D56">
+        <v>3</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C57" s="10">
+        <v>50</v>
+      </c>
+      <c r="D57">
+        <v>3</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C58" s="10">
+        <v>50</v>
+      </c>
+      <c r="D58">
+        <v>3</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="0"/>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1244,8 +2033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A42D5DFB-A5D4-CF45-89DE-E7557FAEE80C}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1261,10 +2050,10 @@
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>64</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1272,11 +2061,11 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="str">
-        <f>TEXT(F2,"DD/MM/YYYY") &amp; " " &amp; TEXT(G2,"H:MM")</f>
+        <f t="shared" ref="B2:B46" si="0">TEXT(F2,"DD/MM/YYYY") &amp; " " &amp; TEXT(G2,"H:MM")</f>
         <v>01/09/2022 9:00</v>
       </c>
       <c r="C2" s="1" t="str">
-        <f>TEXT(F2,"DD/MM/YYYY") &amp; " " &amp; TEXT(H2,"H:MM")</f>
+        <f t="shared" ref="C2:C46" si="1">TEXT(F2,"DD/MM/YYYY") &amp; " " &amp; TEXT(H2,"H:MM")</f>
         <v>01/09/2022 15:00</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -1297,11 +2086,11 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="str">
-        <f>TEXT(F3,"DD/MM/YYYY") &amp; " " &amp; TEXT(G3,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>02/09/2022 9:00</v>
       </c>
       <c r="C3" s="1" t="str">
-        <f>TEXT(F3,"DD/MM/YYYY") &amp; " " &amp; TEXT(H3,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>02/09/2022 15:00</v>
       </c>
       <c r="F3" s="7">
@@ -1319,11 +2108,11 @@
         <v>1</v>
       </c>
       <c r="B4" s="6" t="str">
-        <f>TEXT(F4,"DD/MM/YYYY") &amp; " " &amp; TEXT(G4,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>03/09/2022 9:00</v>
       </c>
       <c r="C4" s="1" t="str">
-        <f>TEXT(F4,"DD/MM/YYYY") &amp; " " &amp; TEXT(H4,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>03/09/2022 15:00</v>
       </c>
       <c r="F4" s="7">
@@ -1341,11 +2130,11 @@
         <v>1</v>
       </c>
       <c r="B5" s="6" t="str">
-        <f>TEXT(F5,"DD/MM/YYYY") &amp; " " &amp; TEXT(G5,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>04/09/2022 9:00</v>
       </c>
       <c r="C5" s="1" t="str">
-        <f>TEXT(F5,"DD/MM/YYYY") &amp; " " &amp; TEXT(H5,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>04/09/2022 15:00</v>
       </c>
       <c r="F5" s="7">
@@ -1363,11 +2152,11 @@
         <v>1</v>
       </c>
       <c r="B6" s="6" t="str">
-        <f>TEXT(F6,"DD/MM/YYYY") &amp; " " &amp; TEXT(G6,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>08/09/2022 9:00</v>
       </c>
       <c r="C6" s="1" t="str">
-        <f>TEXT(F6,"DD/MM/YYYY") &amp; " " &amp; TEXT(H6,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>08/09/2022 15:00</v>
       </c>
       <c r="F6" s="7">
@@ -1386,11 +2175,11 @@
         <v>1</v>
       </c>
       <c r="B7" s="6" t="str">
-        <f>TEXT(F7,"DD/MM/YYYY") &amp; " " &amp; TEXT(G7,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>09/09/2022 9:00</v>
       </c>
       <c r="C7" s="1" t="str">
-        <f>TEXT(F7,"DD/MM/YYYY") &amp; " " &amp; TEXT(H7,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>09/09/2022 15:00</v>
       </c>
       <c r="F7" s="7">
@@ -1409,15 +2198,15 @@
         <v>1</v>
       </c>
       <c r="B8" s="6" t="str">
-        <f>TEXT(F8,"DD/MM/YYYY") &amp; " " &amp; TEXT(G8,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>10/09/2022 9:00</v>
       </c>
       <c r="C8" s="1" t="str">
-        <f>TEXT(F8,"DD/MM/YYYY") &amp; " " &amp; TEXT(H8,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>10/09/2022 15:00</v>
       </c>
       <c r="F8" s="7">
-        <f t="shared" ref="F8:F17" si="0">F7+1</f>
+        <f t="shared" ref="F8:F9" si="2">F7+1</f>
         <v>44814</v>
       </c>
       <c r="G8" s="8">
@@ -1432,15 +2221,15 @@
         <v>1</v>
       </c>
       <c r="B9" s="6" t="str">
-        <f>TEXT(F9,"DD/MM/YYYY") &amp; " " &amp; TEXT(G9,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>11/09/2022 9:00</v>
       </c>
       <c r="C9" s="1" t="str">
-        <f>TEXT(F9,"DD/MM/YYYY") &amp; " " &amp; TEXT(H9,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>11/09/2022 15:00</v>
       </c>
       <c r="F9" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>44815</v>
       </c>
       <c r="G9" s="8">
@@ -1455,11 +2244,11 @@
         <v>1</v>
       </c>
       <c r="B10" s="6" t="str">
-        <f>TEXT(F10,"DD/MM/YYYY") &amp; " " &amp; TEXT(G10,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>15/09/2022 9:00</v>
       </c>
       <c r="C10" s="1" t="str">
-        <f>TEXT(F10,"DD/MM/YYYY") &amp; " " &amp; TEXT(H10,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>15/09/2022 15:00</v>
       </c>
       <c r="F10" s="7">
@@ -1478,11 +2267,11 @@
         <v>1</v>
       </c>
       <c r="B11" s="6" t="str">
-        <f>TEXT(F11,"DD/MM/YYYY") &amp; " " &amp; TEXT(G11,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>16/09/2022 9:00</v>
       </c>
       <c r="C11" s="1" t="str">
-        <f>TEXT(F11,"DD/MM/YYYY") &amp; " " &amp; TEXT(H11,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>16/09/2022 15:00</v>
       </c>
       <c r="F11" s="7">
@@ -1501,15 +2290,15 @@
         <v>1</v>
       </c>
       <c r="B12" s="6" t="str">
-        <f>TEXT(F12,"DD/MM/YYYY") &amp; " " &amp; TEXT(G12,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>17/09/2022 9:00</v>
       </c>
       <c r="C12" s="1" t="str">
-        <f>TEXT(F12,"DD/MM/YYYY") &amp; " " &amp; TEXT(H12,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>17/09/2022 15:00</v>
       </c>
       <c r="F12" s="7">
-        <f t="shared" ref="F12:F21" si="1">F11+1</f>
+        <f t="shared" ref="F12:F13" si="3">F11+1</f>
         <v>44821</v>
       </c>
       <c r="G12" s="8">
@@ -1524,15 +2313,15 @@
         <v>1</v>
       </c>
       <c r="B13" s="6" t="str">
-        <f>TEXT(F13,"DD/MM/YYYY") &amp; " " &amp; TEXT(G13,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>18/09/2022 9:00</v>
       </c>
       <c r="C13" s="1" t="str">
-        <f>TEXT(F13,"DD/MM/YYYY") &amp; " " &amp; TEXT(H13,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>18/09/2022 15:00</v>
       </c>
       <c r="F13" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44822</v>
       </c>
       <c r="G13" s="8">
@@ -1547,11 +2336,11 @@
         <v>1</v>
       </c>
       <c r="B14" s="6" t="str">
-        <f>TEXT(F14,"DD/MM/YYYY") &amp; " " &amp; TEXT(G14,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>22/09/2022 9:00</v>
       </c>
       <c r="C14" s="1" t="str">
-        <f>TEXT(F14,"DD/MM/YYYY") &amp; " " &amp; TEXT(H14,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>22/09/2022 15:00</v>
       </c>
       <c r="F14" s="7">
@@ -1570,11 +2359,11 @@
         <v>1</v>
       </c>
       <c r="B15" s="6" t="str">
-        <f>TEXT(F15,"DD/MM/YYYY") &amp; " " &amp; TEXT(G15,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>23/09/2022 9:00</v>
       </c>
       <c r="C15" s="1" t="str">
-        <f>TEXT(F15,"DD/MM/YYYY") &amp; " " &amp; TEXT(H15,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>23/09/2022 15:00</v>
       </c>
       <c r="F15" s="7">
@@ -1593,15 +2382,15 @@
         <v>1</v>
       </c>
       <c r="B16" s="6" t="str">
-        <f>TEXT(F16,"DD/MM/YYYY") &amp; " " &amp; TEXT(G16,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>24/09/2022 9:00</v>
       </c>
       <c r="C16" s="1" t="str">
-        <f>TEXT(F16,"DD/MM/YYYY") &amp; " " &amp; TEXT(H16,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>24/09/2022 15:00</v>
       </c>
       <c r="F16" s="7">
-        <f t="shared" ref="F16:F21" si="2">F15+1</f>
+        <f t="shared" ref="F16:F17" si="4">F15+1</f>
         <v>44828</v>
       </c>
       <c r="G16" s="8">
@@ -1616,15 +2405,15 @@
         <v>1</v>
       </c>
       <c r="B17" s="6" t="str">
-        <f>TEXT(F17,"DD/MM/YYYY") &amp; " " &amp; TEXT(G17,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>25/09/2022 9:00</v>
       </c>
       <c r="C17" s="1" t="str">
-        <f>TEXT(F17,"DD/MM/YYYY") &amp; " " &amp; TEXT(H17,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>25/09/2022 15:00</v>
       </c>
       <c r="F17" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44829</v>
       </c>
       <c r="G17" s="8">
@@ -1639,11 +2428,11 @@
         <v>1</v>
       </c>
       <c r="B18" s="6" t="str">
-        <f>TEXT(F18,"DD/MM/YYYY") &amp; " " &amp; TEXT(G18,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>29/09/2022 9:00</v>
       </c>
       <c r="C18" s="1" t="str">
-        <f>TEXT(F18,"DD/MM/YYYY") &amp; " " &amp; TEXT(H18,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>29/09/2022 15:00</v>
       </c>
       <c r="F18" s="7">
@@ -1662,11 +2451,11 @@
         <v>1</v>
       </c>
       <c r="B19" s="6" t="str">
-        <f>TEXT(F19,"DD/MM/YYYY") &amp; " " &amp; TEXT(G19,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>30/09/2022 9:00</v>
       </c>
       <c r="C19" s="1" t="str">
-        <f>TEXT(F19,"DD/MM/YYYY") &amp; " " &amp; TEXT(H19,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>30/09/2022 15:00</v>
       </c>
       <c r="F19" s="7">
@@ -1685,15 +2474,15 @@
         <v>1</v>
       </c>
       <c r="B20" s="6" t="str">
-        <f>TEXT(F20,"DD/MM/YYYY") &amp; " " &amp; TEXT(G20,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>01/10/2022 9:00</v>
       </c>
       <c r="C20" s="1" t="str">
-        <f>TEXT(F20,"DD/MM/YYYY") &amp; " " &amp; TEXT(H20,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>01/10/2022 15:00</v>
       </c>
       <c r="F20" s="7">
-        <f t="shared" ref="F20:F21" si="3">F19+1</f>
+        <f t="shared" ref="F20:F21" si="5">F19+1</f>
         <v>44835</v>
       </c>
       <c r="G20" s="8">
@@ -1708,15 +2497,15 @@
         <v>1</v>
       </c>
       <c r="B21" s="6" t="str">
-        <f>TEXT(F21,"DD/MM/YYYY") &amp; " " &amp; TEXT(G21,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>02/10/2022 9:00</v>
       </c>
       <c r="C21" s="1" t="str">
-        <f>TEXT(F21,"DD/MM/YYYY") &amp; " " &amp; TEXT(H21,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>02/10/2022 15:00</v>
       </c>
       <c r="F21" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>44836</v>
       </c>
       <c r="G21" s="8">
@@ -1731,11 +2520,11 @@
         <v>2</v>
       </c>
       <c r="B22" s="5" t="str">
-        <f>TEXT(F22,"DD/MM/YYYY") &amp; " " &amp; TEXT(G22,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>03/09/2022 8:00</v>
       </c>
       <c r="C22" t="str">
-        <f>TEXT(F22,"DD/MM/YYYY") &amp; " " &amp; TEXT(H22,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>03/09/2022 13:30</v>
       </c>
       <c r="E22" t="s">
@@ -1756,11 +2545,11 @@
         <v>2</v>
       </c>
       <c r="B23" s="5" t="str">
-        <f>TEXT(F23,"DD/MM/YYYY") &amp; " " &amp; TEXT(G23,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>04/09/2022 8:00</v>
       </c>
       <c r="C23" t="str">
-        <f>TEXT(F23,"DD/MM/YYYY") &amp; " " &amp; TEXT(H23,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>04/09/2022 13:30</v>
       </c>
       <c r="F23" s="4">
@@ -1779,11 +2568,11 @@
         <v>2</v>
       </c>
       <c r="B24" s="5" t="str">
-        <f>TEXT(F24,"DD/MM/YYYY") &amp; " " &amp; TEXT(G24,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>10/09/2022 8:00</v>
       </c>
       <c r="C24" t="str">
-        <f>TEXT(F24,"DD/MM/YYYY") &amp; " " &amp; TEXT(H24,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>10/09/2022 13:30</v>
       </c>
       <c r="F24" s="4">
@@ -1802,11 +2591,11 @@
         <v>2</v>
       </c>
       <c r="B25" s="5" t="str">
-        <f>TEXT(F25,"DD/MM/YYYY") &amp; " " &amp; TEXT(G25,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>11/09/2022 8:00</v>
       </c>
       <c r="C25" t="str">
-        <f>TEXT(F25,"DD/MM/YYYY") &amp; " " &amp; TEXT(H25,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>11/09/2022 13:30</v>
       </c>
       <c r="F25" s="4">
@@ -1825,11 +2614,11 @@
         <v>2</v>
       </c>
       <c r="B26" s="5" t="str">
-        <f>TEXT(F26,"DD/MM/YYYY") &amp; " " &amp; TEXT(G26,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>17/09/2022 8:00</v>
       </c>
       <c r="C26" t="str">
-        <f>TEXT(F26,"DD/MM/YYYY") &amp; " " &amp; TEXT(H26,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>17/09/2022 13:30</v>
       </c>
       <c r="F26" s="4">
@@ -1848,11 +2637,11 @@
         <v>2</v>
       </c>
       <c r="B27" s="5" t="str">
-        <f>TEXT(F27,"DD/MM/YYYY") &amp; " " &amp; TEXT(G27,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>18/09/2022 8:00</v>
       </c>
       <c r="C27" t="str">
-        <f>TEXT(F27,"DD/MM/YYYY") &amp; " " &amp; TEXT(H27,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>18/09/2022 13:30</v>
       </c>
       <c r="F27" s="4">
@@ -1871,11 +2660,11 @@
         <v>2</v>
       </c>
       <c r="B28" s="5" t="str">
-        <f>TEXT(F28,"DD/MM/YYYY") &amp; " " &amp; TEXT(G28,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>24/09/2022 8:00</v>
       </c>
       <c r="C28" t="str">
-        <f>TEXT(F28,"DD/MM/YYYY") &amp; " " &amp; TEXT(H28,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>24/09/2022 13:30</v>
       </c>
       <c r="F28" s="4">
@@ -1894,11 +2683,11 @@
         <v>2</v>
       </c>
       <c r="B29" s="5" t="str">
-        <f>TEXT(F29,"DD/MM/YYYY") &amp; " " &amp; TEXT(G29,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>25/09/2022 8:00</v>
       </c>
       <c r="C29" t="str">
-        <f>TEXT(F29,"DD/MM/YYYY") &amp; " " &amp; TEXT(H29,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>25/09/2022 13:30</v>
       </c>
       <c r="F29" s="4">
@@ -1917,11 +2706,11 @@
         <v>2</v>
       </c>
       <c r="B30" s="5" t="str">
-        <f>TEXT(F30,"DD/MM/YYYY") &amp; " " &amp; TEXT(G30,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>01/10/2022 8:00</v>
       </c>
       <c r="C30" t="str">
-        <f>TEXT(F30,"DD/MM/YYYY") &amp; " " &amp; TEXT(H30,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>01/10/2022 13:30</v>
       </c>
       <c r="F30" s="4">
@@ -1940,11 +2729,11 @@
         <v>2</v>
       </c>
       <c r="B31" s="5" t="str">
-        <f>TEXT(F31,"DD/MM/YYYY") &amp; " " &amp; TEXT(G31,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>02/10/2022 8:00</v>
       </c>
       <c r="C31" t="str">
-        <f>TEXT(F31,"DD/MM/YYYY") &amp; " " &amp; TEXT(H31,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>02/10/2022 13:30</v>
       </c>
       <c r="F31" s="4">
@@ -1963,11 +2752,11 @@
         <v>2</v>
       </c>
       <c r="B32" s="5" t="str">
-        <f>TEXT(F32,"DD/MM/YYYY") &amp; " " &amp; TEXT(G32,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>08/10/2022 8:00</v>
       </c>
       <c r="C32" t="str">
-        <f>TEXT(F32,"DD/MM/YYYY") &amp; " " &amp; TEXT(H32,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>08/10/2022 13:30</v>
       </c>
       <c r="F32" s="4">
@@ -1986,11 +2775,11 @@
         <v>2</v>
       </c>
       <c r="B33" s="5" t="str">
-        <f>TEXT(F33,"DD/MM/YYYY") &amp; " " &amp; TEXT(G33,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>09/10/2022 8:00</v>
       </c>
       <c r="C33" t="str">
-        <f>TEXT(F33,"DD/MM/YYYY") &amp; " " &amp; TEXT(H33,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>09/10/2022 13:30</v>
       </c>
       <c r="F33" s="4">
@@ -2009,11 +2798,11 @@
         <v>3</v>
       </c>
       <c r="B34" s="5" t="str">
-        <f>TEXT(F34,"DD/MM/YYYY") &amp; " " &amp; TEXT(G34,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>15/10/2022 8:00</v>
       </c>
       <c r="C34" t="str">
-        <f>TEXT(F34,"DD/MM/YYYY") &amp; " " &amp; TEXT(H34,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>15/10/2022 13:30</v>
       </c>
       <c r="F34" s="4">
@@ -2032,11 +2821,11 @@
         <v>3</v>
       </c>
       <c r="B35" s="5" t="str">
-        <f>TEXT(F35,"DD/MM/YYYY") &amp; " " &amp; TEXT(G35,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>16/10/2022 8:00</v>
       </c>
       <c r="C35" t="str">
-        <f>TEXT(F35,"DD/MM/YYYY") &amp; " " &amp; TEXT(H35,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>16/10/2022 13:30</v>
       </c>
       <c r="F35" s="4">
@@ -2055,11 +2844,11 @@
         <v>3</v>
       </c>
       <c r="B36" s="5" t="str">
-        <f>TEXT(F36,"DD/MM/YYYY") &amp; " " &amp; TEXT(G36,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>22/10/2022 8:00</v>
       </c>
       <c r="C36" t="str">
-        <f>TEXT(F36,"DD/MM/YYYY") &amp; " " &amp; TEXT(H36,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>22/10/2022 13:30</v>
       </c>
       <c r="F36" s="4">
@@ -2078,11 +2867,11 @@
         <v>3</v>
       </c>
       <c r="B37" s="5" t="str">
-        <f>TEXT(F37,"DD/MM/YYYY") &amp; " " &amp; TEXT(G37,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>23/10/2022 8:00</v>
       </c>
       <c r="C37" t="str">
-        <f>TEXT(F37,"DD/MM/YYYY") &amp; " " &amp; TEXT(H37,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>23/10/2022 13:30</v>
       </c>
       <c r="F37" s="4">
@@ -2101,11 +2890,11 @@
         <v>3</v>
       </c>
       <c r="B38" s="5" t="str">
-        <f>TEXT(F38,"DD/MM/YYYY") &amp; " " &amp; TEXT(G38,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>29/10/2022 8:00</v>
       </c>
       <c r="C38" t="str">
-        <f>TEXT(F38,"DD/MM/YYYY") &amp; " " &amp; TEXT(H38,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>29/10/2022 13:30</v>
       </c>
       <c r="F38" s="4">
@@ -2124,11 +2913,11 @@
         <v>3</v>
       </c>
       <c r="B39" s="5" t="str">
-        <f>TEXT(F39,"DD/MM/YYYY") &amp; " " &amp; TEXT(G39,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>30/10/2022 8:00</v>
       </c>
       <c r="C39" t="str">
-        <f>TEXT(F39,"DD/MM/YYYY") &amp; " " &amp; TEXT(H39,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>30/10/2022 13:30</v>
       </c>
       <c r="F39" s="4">
@@ -2147,11 +2936,11 @@
         <v>3</v>
       </c>
       <c r="B40" s="5" t="str">
-        <f>TEXT(F40,"DD/MM/YYYY") &amp; " " &amp; TEXT(G40,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>05/11/2022 8:00</v>
       </c>
       <c r="C40" t="str">
-        <f>TEXT(F40,"DD/MM/YYYY") &amp; " " &amp; TEXT(H40,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>05/11/2022 13:30</v>
       </c>
       <c r="F40" s="4">
@@ -2170,11 +2959,11 @@
         <v>3</v>
       </c>
       <c r="B41" s="5" t="str">
-        <f>TEXT(F41,"DD/MM/YYYY") &amp; " " &amp; TEXT(G41,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>06/11/2022 8:00</v>
       </c>
       <c r="C41" t="str">
-        <f>TEXT(F41,"DD/MM/YYYY") &amp; " " &amp; TEXT(H41,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>06/11/2022 13:30</v>
       </c>
       <c r="F41" s="4">
@@ -2193,11 +2982,11 @@
         <v>3</v>
       </c>
       <c r="B42" s="6" t="str">
-        <f>TEXT(F42,"DD/MM/YYYY") &amp; " " &amp; TEXT(G42,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>02/10/2022 7:30</v>
       </c>
       <c r="C42" s="1" t="str">
-        <f>TEXT(F42,"DD/MM/YYYY") &amp; " " &amp; TEXT(H42,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>02/10/2022 14:00</v>
       </c>
       <c r="E42" s="1" t="s">
@@ -2219,11 +3008,11 @@
         <v>3</v>
       </c>
       <c r="B43" s="6" t="str">
-        <f>TEXT(F43,"DD/MM/YYYY") &amp; " " &amp; TEXT(G43,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>30/10/2022 7:30</v>
       </c>
       <c r="C43" s="1" t="str">
-        <f>TEXT(F43,"DD/MM/YYYY") &amp; " " &amp; TEXT(H43,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>30/10/2022 14:00</v>
       </c>
       <c r="F43" s="7">
@@ -2242,11 +3031,11 @@
         <v>3</v>
       </c>
       <c r="B44" s="6" t="str">
-        <f>TEXT(F44,"DD/MM/YYYY") &amp; " " &amp; TEXT(G44,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>04/12/2022 7:30</v>
       </c>
       <c r="C44" s="1" t="str">
-        <f>TEXT(F44,"DD/MM/YYYY") &amp; " " &amp; TEXT(H44,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>04/12/2022 14:00</v>
       </c>
       <c r="F44" s="7">
@@ -2265,15 +3054,15 @@
         <v>3</v>
       </c>
       <c r="B45" s="6" t="str">
-        <f>TEXT(F45,"DD/MM/YYYY") &amp; " " &amp; TEXT(G45,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>01/01/2023 7:30</v>
       </c>
       <c r="C45" s="1" t="str">
-        <f>TEXT(F45,"DD/MM/YYYY") &amp; " " &amp; TEXT(H45,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>01/01/2023 14:00</v>
       </c>
       <c r="F45" s="7">
-        <f t="shared" ref="F45:F46" si="4">F44+28</f>
+        <f t="shared" ref="F45" si="6">F44+28</f>
         <v>44927</v>
       </c>
       <c r="G45" s="8">
@@ -2288,11 +3077,11 @@
         <v>3</v>
       </c>
       <c r="B46" s="6" t="str">
-        <f>TEXT(F46,"DD/MM/YYYY") &amp; " " &amp; TEXT(G46,"H:MM")</f>
+        <f t="shared" si="0"/>
         <v>05/02/2023 7:30</v>
       </c>
       <c r="C46" s="1" t="str">
-        <f>TEXT(F46,"DD/MM/YYYY") &amp; " " &amp; TEXT(H46,"H:MM")</f>
+        <f t="shared" si="1"/>
         <v>05/02/2023 14:00</v>
       </c>
       <c r="F46" s="7">
@@ -2305,6 +3094,2486 @@
       <c r="H46" s="8">
         <v>0.58333333333333304</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7346D73A-D93A-C84C-8558-1A5ED94E4EFB}">
+  <dimension ref="A1:V58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="Q1" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="S1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="T1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="U1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="V1" s="9"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="11">
+        <v>1</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="M2" s="14">
+        <v>44805</v>
+      </c>
+      <c r="N2" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="O2" s="15">
+        <v>0.625</v>
+      </c>
+      <c r="Q2" s="9">
+        <v>1</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="T2" s="9">
+        <v>30</v>
+      </c>
+      <c r="U2" s="9">
+        <v>1</v>
+      </c>
+      <c r="V2" s="9"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" t="s">
+        <v>168</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3" s="11">
+        <v>1</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="14">
+        <v>44806</v>
+      </c>
+      <c r="N3" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="O3" s="15">
+        <v>0.625</v>
+      </c>
+      <c r="Q3" s="9">
+        <f>Q2+1</f>
+        <v>2</v>
+      </c>
+      <c r="R3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="S3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="T3" s="9">
+        <v>30</v>
+      </c>
+      <c r="U3" s="9">
+        <v>1</v>
+      </c>
+      <c r="V3" s="9"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4" s="11">
+        <v>1</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="14">
+        <v>44807</v>
+      </c>
+      <c r="N4" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="O4" s="15">
+        <v>0.625</v>
+      </c>
+      <c r="Q4" s="9">
+        <f t="shared" ref="Q4:Q58" si="0">Q3+1</f>
+        <v>3</v>
+      </c>
+      <c r="R4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="S4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="T4" s="9">
+        <v>30</v>
+      </c>
+      <c r="U4" s="9">
+        <v>1</v>
+      </c>
+      <c r="V4" s="9"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5" s="11">
+        <v>1</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="14">
+        <v>44808</v>
+      </c>
+      <c r="N5" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="O5" s="15">
+        <v>0.625</v>
+      </c>
+      <c r="Q5" s="9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="R5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="S5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="T5" s="9">
+        <v>30</v>
+      </c>
+      <c r="U5" s="9">
+        <v>1</v>
+      </c>
+      <c r="V5" s="9"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>21</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="E6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6" s="11">
+        <v>1</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="14">
+        <f>M2+7</f>
+        <v>44812</v>
+      </c>
+      <c r="N6" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="O6" s="15">
+        <v>0.625</v>
+      </c>
+      <c r="Q6" s="9">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="R6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="S6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="T6" s="9">
+        <v>45</v>
+      </c>
+      <c r="U6" s="9">
+        <v>1</v>
+      </c>
+      <c r="V6" s="9"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>22</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="E7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7" s="11">
+        <v>1</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="14">
+        <f>M6+1</f>
+        <v>44813</v>
+      </c>
+      <c r="N7" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="O7" s="15">
+        <v>0.625</v>
+      </c>
+      <c r="Q7" s="9">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="R7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="S7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="T7" s="9">
+        <v>45</v>
+      </c>
+      <c r="U7" s="9">
+        <v>1</v>
+      </c>
+      <c r="V7" s="9"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>41</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="E8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8">
+        <v>7</v>
+      </c>
+      <c r="H8" s="11">
+        <v>1</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="14">
+        <f t="shared" ref="M8:M9" si="1">M7+1</f>
+        <v>44814</v>
+      </c>
+      <c r="N8" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="O8" s="15">
+        <v>0.625</v>
+      </c>
+      <c r="Q8" s="9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="R8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="S8" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="T8" s="9">
+        <v>45</v>
+      </c>
+      <c r="U8" s="9">
+        <v>1</v>
+      </c>
+      <c r="V8" s="9"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>42</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="E9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9" s="11">
+        <v>1</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="14">
+        <f t="shared" si="1"/>
+        <v>44815</v>
+      </c>
+      <c r="N9" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="O9" s="15">
+        <v>0.625</v>
+      </c>
+      <c r="Q9" s="9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="R9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="S9" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="T9" s="9">
+        <v>45</v>
+      </c>
+      <c r="U9" s="9">
+        <v>1</v>
+      </c>
+      <c r="V9" s="9"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="C10" s="23"/>
+      <c r="G10">
+        <v>9</v>
+      </c>
+      <c r="H10" s="11">
+        <v>1</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="14">
+        <f>M6+7</f>
+        <v>44819</v>
+      </c>
+      <c r="N10" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="O10" s="15">
+        <v>0.625</v>
+      </c>
+      <c r="Q10" s="9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="R10" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="S10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="T10" s="9">
+        <v>45</v>
+      </c>
+      <c r="U10" s="9">
+        <v>1</v>
+      </c>
+      <c r="V10" s="9"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11" s="11">
+        <v>1</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="14">
+        <f>M10+1</f>
+        <v>44820</v>
+      </c>
+      <c r="N11" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="O11" s="15">
+        <v>0.625</v>
+      </c>
+      <c r="Q11" s="9">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="R11" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="S11" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="T11" s="9">
+        <v>45</v>
+      </c>
+      <c r="U11" s="9">
+        <v>1</v>
+      </c>
+      <c r="V11" s="9"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12">
+        <v>11</v>
+      </c>
+      <c r="H12" s="11">
+        <v>1</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="14">
+        <f t="shared" ref="M12:M13" si="2">M11+1</f>
+        <v>44821</v>
+      </c>
+      <c r="N12" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="O12" s="15">
+        <v>0.625</v>
+      </c>
+      <c r="Q12" s="9">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="R12" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="S12" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="T12" s="9">
+        <v>50</v>
+      </c>
+      <c r="U12" s="9">
+        <v>1</v>
+      </c>
+      <c r="V12" s="9"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" t="s">
+        <v>77</v>
+      </c>
+      <c r="G13">
+        <v>12</v>
+      </c>
+      <c r="H13" s="11">
+        <v>1</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="14">
+        <f t="shared" si="2"/>
+        <v>44822</v>
+      </c>
+      <c r="N13" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="O13" s="15">
+        <v>0.625</v>
+      </c>
+      <c r="Q13" s="9">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="R13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="S13" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="T13" s="9">
+        <v>50</v>
+      </c>
+      <c r="U13" s="9">
+        <v>1</v>
+      </c>
+      <c r="V13" s="9"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="21">
+        <v>1</v>
+      </c>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="G14">
+        <v>13</v>
+      </c>
+      <c r="H14" s="11">
+        <v>1</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="14">
+        <f>M10+7</f>
+        <v>44826</v>
+      </c>
+      <c r="N14" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="O14" s="15">
+        <v>0.625</v>
+      </c>
+      <c r="Q14" s="9">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="R14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="S14" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="T14" s="9">
+        <v>50</v>
+      </c>
+      <c r="U14" s="9">
+        <v>1</v>
+      </c>
+      <c r="V14" s="9"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" s="21">
+        <f>IF(B15=B14,C14,C14+1)</f>
+        <v>1</v>
+      </c>
+      <c r="D15" s="22"/>
+      <c r="E15" s="21"/>
+      <c r="G15">
+        <v>14</v>
+      </c>
+      <c r="H15" s="11">
+        <v>1</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="14">
+        <f>M14+1</f>
+        <v>44827</v>
+      </c>
+      <c r="N15" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="O15" s="15">
+        <v>0.625</v>
+      </c>
+      <c r="Q15" s="9">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="R15" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="S15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="T15" s="9">
+        <v>55</v>
+      </c>
+      <c r="U15" s="9">
+        <v>1</v>
+      </c>
+      <c r="V15" s="9"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="21">
+        <f t="shared" ref="C16:C25" si="3">IF(B16=B15,C15,C15+1)</f>
+        <v>1</v>
+      </c>
+      <c r="D16" s="22"/>
+      <c r="E16" s="21"/>
+      <c r="G16">
+        <v>15</v>
+      </c>
+      <c r="H16" s="11">
+        <v>1</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="14">
+        <f t="shared" ref="M16:M17" si="4">M15+1</f>
+        <v>44828</v>
+      </c>
+      <c r="N16" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="O16" s="15">
+        <v>0.625</v>
+      </c>
+      <c r="Q16" s="9">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="R16" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="S16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="T16" s="9">
+        <v>55</v>
+      </c>
+      <c r="U16" s="9">
+        <v>1</v>
+      </c>
+      <c r="V16" s="9"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" s="21">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D17" s="22"/>
+      <c r="E17" s="21"/>
+      <c r="G17">
+        <v>16</v>
+      </c>
+      <c r="H17" s="11">
+        <v>1</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="14">
+        <f t="shared" si="4"/>
+        <v>44829</v>
+      </c>
+      <c r="N17" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="O17" s="15">
+        <v>0.625</v>
+      </c>
+      <c r="Q17" s="9">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="R17" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="S17" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="T17" s="9">
+        <v>120</v>
+      </c>
+      <c r="U17" s="9">
+        <v>1</v>
+      </c>
+      <c r="V17" s="9"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <v>21</v>
+      </c>
+      <c r="C18" s="21">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="D18" s="22"/>
+      <c r="E18" s="21"/>
+      <c r="G18">
+        <v>17</v>
+      </c>
+      <c r="H18" s="11">
+        <v>1</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="14">
+        <f>M14+7</f>
+        <v>44833</v>
+      </c>
+      <c r="N18" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="O18" s="15">
+        <v>0.625</v>
+      </c>
+      <c r="Q18" s="9">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="R18" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="S18" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="T18" s="9">
+        <v>100</v>
+      </c>
+      <c r="U18" s="9">
+        <v>1</v>
+      </c>
+      <c r="V18" s="9"/>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <v>21</v>
+      </c>
+      <c r="C19" s="21">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="G19">
+        <v>18</v>
+      </c>
+      <c r="H19" s="11">
+        <v>1</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="J19" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="14">
+        <f>M18+1</f>
+        <v>44834</v>
+      </c>
+      <c r="N19" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="O19" s="15">
+        <v>0.625</v>
+      </c>
+      <c r="Q19" s="9">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="R19" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="S19" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="T19" s="9">
+        <v>120</v>
+      </c>
+      <c r="U19" s="9">
+        <v>1</v>
+      </c>
+      <c r="V19" s="9"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>23</v>
+      </c>
+      <c r="B20">
+        <v>21</v>
+      </c>
+      <c r="C20" s="21">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="G20">
+        <v>19</v>
+      </c>
+      <c r="H20" s="11">
+        <v>1</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="J20" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="14">
+        <f t="shared" ref="M20:M21" si="5">M19+1</f>
+        <v>44835</v>
+      </c>
+      <c r="N20" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="O20" s="15">
+        <v>0.625</v>
+      </c>
+      <c r="Q20" s="9">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="R20" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="S20" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="T20" s="9">
+        <v>90</v>
+      </c>
+      <c r="U20" s="9">
+        <v>1</v>
+      </c>
+      <c r="V20" s="9"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>22</v>
+      </c>
+      <c r="B21">
+        <v>22</v>
+      </c>
+      <c r="C21" s="21">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="G21">
+        <v>20</v>
+      </c>
+      <c r="H21" s="11">
+        <v>1</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="J21" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="14">
+        <f t="shared" si="5"/>
+        <v>44836</v>
+      </c>
+      <c r="N21" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="O21" s="15">
+        <v>0.625</v>
+      </c>
+      <c r="Q21" s="9">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="R21" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="S21" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="T21" s="9">
+        <v>120</v>
+      </c>
+      <c r="U21" s="9">
+        <v>1</v>
+      </c>
+      <c r="V21" s="9"/>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>41</v>
+      </c>
+      <c r="B22">
+        <v>41</v>
+      </c>
+      <c r="C22" s="21">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="G22" s="16">
+        <v>21</v>
+      </c>
+      <c r="H22" s="17">
+        <v>2</v>
+      </c>
+      <c r="I22" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="J22" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="M22" s="19">
+        <v>44807</v>
+      </c>
+      <c r="N22" s="20">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="O22" s="20">
+        <v>0.5625</v>
+      </c>
+      <c r="Q22" s="9">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="R22" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="S22" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="T22" s="9">
+        <v>90</v>
+      </c>
+      <c r="U22" s="9">
+        <v>1</v>
+      </c>
+      <c r="V22" s="9"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>42</v>
+      </c>
+      <c r="B23">
+        <v>41</v>
+      </c>
+      <c r="C23" s="21">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="G23">
+        <v>22</v>
+      </c>
+      <c r="H23" s="11">
+        <v>2</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="J23" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="14">
+        <f>M22+1</f>
+        <v>44808</v>
+      </c>
+      <c r="N23" s="15">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="O23" s="15">
+        <v>0.5625</v>
+      </c>
+      <c r="Q23" s="9">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="R23" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="S23" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="T23" s="9">
+        <v>25</v>
+      </c>
+      <c r="U23" s="9">
+        <v>2</v>
+      </c>
+      <c r="V23" s="9"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>43</v>
+      </c>
+      <c r="B24">
+        <v>41</v>
+      </c>
+      <c r="C24" s="21">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="G24">
+        <v>23</v>
+      </c>
+      <c r="H24" s="11">
+        <v>2</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="J24" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="14">
+        <f>M22+7</f>
+        <v>44814</v>
+      </c>
+      <c r="N24" s="15">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="O24" s="15">
+        <v>0.5625</v>
+      </c>
+      <c r="Q24" s="9">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="R24" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="S24" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="T24" s="9">
+        <v>25</v>
+      </c>
+      <c r="U24" s="9">
+        <v>2</v>
+      </c>
+      <c r="V24" s="9"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>42</v>
+      </c>
+      <c r="B25">
+        <v>42</v>
+      </c>
+      <c r="C25" s="21">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="G25">
+        <v>24</v>
+      </c>
+      <c r="H25" s="11">
+        <v>2</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="J25" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="14">
+        <f>M24+1</f>
+        <v>44815</v>
+      </c>
+      <c r="N25" s="15">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="O25" s="15">
+        <v>0.5625</v>
+      </c>
+      <c r="Q25" s="9">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="R25" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="S25" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="T25" s="9">
+        <v>25</v>
+      </c>
+      <c r="U25" s="9">
+        <v>2</v>
+      </c>
+      <c r="V25" s="9"/>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="G26">
+        <v>25</v>
+      </c>
+      <c r="H26" s="11">
+        <v>2</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="J26" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="14">
+        <f>M24+7</f>
+        <v>44821</v>
+      </c>
+      <c r="N26" s="15">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="O26" s="15">
+        <v>0.5625</v>
+      </c>
+      <c r="Q26" s="9">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="R26" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="S26" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="T26" s="9">
+        <v>25</v>
+      </c>
+      <c r="U26" s="9">
+        <v>2</v>
+      </c>
+      <c r="V26" s="9"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="G27">
+        <v>26</v>
+      </c>
+      <c r="H27" s="11">
+        <v>2</v>
+      </c>
+      <c r="I27" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="J27" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="14">
+        <f>M26+1</f>
+        <v>44822</v>
+      </c>
+      <c r="N27" s="15">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="O27" s="15">
+        <v>0.5625</v>
+      </c>
+      <c r="Q27" s="9">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="R27" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="S27" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="T27" s="9">
+        <v>40</v>
+      </c>
+      <c r="U27" s="9">
+        <v>2</v>
+      </c>
+      <c r="V27" s="9"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="G28">
+        <v>27</v>
+      </c>
+      <c r="H28" s="11">
+        <v>2</v>
+      </c>
+      <c r="I28" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="J28" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="14">
+        <f>M26+7</f>
+        <v>44828</v>
+      </c>
+      <c r="N28" s="15">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="O28" s="15">
+        <v>0.5625</v>
+      </c>
+      <c r="Q28" s="9">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="R28" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="S28" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="T28" s="9">
+        <v>40</v>
+      </c>
+      <c r="U28" s="9">
+        <v>2</v>
+      </c>
+      <c r="V28" s="9"/>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="G29">
+        <v>28</v>
+      </c>
+      <c r="H29" s="11">
+        <v>2</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="J29" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="14">
+        <f>M28+1</f>
+        <v>44829</v>
+      </c>
+      <c r="N29" s="15">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="O29" s="15">
+        <v>0.5625</v>
+      </c>
+      <c r="Q29" s="9">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="R29" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="S29" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="T29" s="9">
+        <v>40</v>
+      </c>
+      <c r="U29" s="9">
+        <v>2</v>
+      </c>
+      <c r="V29" s="9"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="G30">
+        <v>29</v>
+      </c>
+      <c r="H30" s="11">
+        <v>2</v>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="J30" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="14">
+        <f>M28+7</f>
+        <v>44835</v>
+      </c>
+      <c r="N30" s="15">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="O30" s="15">
+        <v>0.5625</v>
+      </c>
+      <c r="Q30" s="9">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="R30" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="S30" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="T30" s="9">
+        <v>40</v>
+      </c>
+      <c r="U30" s="9">
+        <v>2</v>
+      </c>
+      <c r="V30" s="9"/>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="G31">
+        <v>30</v>
+      </c>
+      <c r="H31" s="11">
+        <v>2</v>
+      </c>
+      <c r="I31" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="J31" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="14">
+        <f>M30+1</f>
+        <v>44836</v>
+      </c>
+      <c r="N31" s="15">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="O31" s="15">
+        <v>0.5625</v>
+      </c>
+      <c r="Q31" s="9">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="R31" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="S31" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="T31" s="9">
+        <v>40</v>
+      </c>
+      <c r="U31" s="9">
+        <v>2</v>
+      </c>
+      <c r="V31" s="9"/>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="G32">
+        <v>31</v>
+      </c>
+      <c r="H32" s="11">
+        <v>2</v>
+      </c>
+      <c r="I32" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="J32" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="14">
+        <f>M30+7</f>
+        <v>44842</v>
+      </c>
+      <c r="N32" s="15">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="O32" s="15">
+        <v>0.5625</v>
+      </c>
+      <c r="Q32" s="9">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="R32" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="S32" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="T32" s="9">
+        <v>40</v>
+      </c>
+      <c r="U32" s="9">
+        <v>2</v>
+      </c>
+      <c r="V32" s="9"/>
+    </row>
+    <row r="33" spans="7:22" x14ac:dyDescent="0.2">
+      <c r="G33">
+        <v>32</v>
+      </c>
+      <c r="H33" s="11">
+        <v>2</v>
+      </c>
+      <c r="I33" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="J33" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="14">
+        <f>M32+1</f>
+        <v>44843</v>
+      </c>
+      <c r="N33" s="15">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="O33" s="15">
+        <v>0.5625</v>
+      </c>
+      <c r="Q33" s="9">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="R33" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="S33" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="T33" s="9">
+        <v>45</v>
+      </c>
+      <c r="U33" s="9">
+        <v>2</v>
+      </c>
+      <c r="V33" s="9"/>
+    </row>
+    <row r="34" spans="7:22" x14ac:dyDescent="0.2">
+      <c r="G34">
+        <v>33</v>
+      </c>
+      <c r="H34" s="11">
+        <v>3</v>
+      </c>
+      <c r="I34" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="J34" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="14">
+        <f>M32+7</f>
+        <v>44849</v>
+      </c>
+      <c r="N34" s="15">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="O34" s="15">
+        <v>0.5625</v>
+      </c>
+      <c r="Q34" s="9">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="R34" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="S34" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="T34" s="9">
+        <v>45</v>
+      </c>
+      <c r="U34" s="9">
+        <v>2</v>
+      </c>
+      <c r="V34" s="9"/>
+    </row>
+    <row r="35" spans="7:22" x14ac:dyDescent="0.2">
+      <c r="G35">
+        <v>34</v>
+      </c>
+      <c r="H35" s="11">
+        <v>3</v>
+      </c>
+      <c r="I35" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="J35" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="K35" s="11"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="14">
+        <f>M34+1</f>
+        <v>44850</v>
+      </c>
+      <c r="N35" s="15">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="O35" s="15">
+        <v>0.5625</v>
+      </c>
+      <c r="Q35" s="9">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="R35" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="S35" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="T35" s="9">
+        <v>45</v>
+      </c>
+      <c r="U35" s="9">
+        <v>2</v>
+      </c>
+      <c r="V35" s="9"/>
+    </row>
+    <row r="36" spans="7:22" x14ac:dyDescent="0.2">
+      <c r="G36">
+        <v>35</v>
+      </c>
+      <c r="H36" s="11">
+        <v>3</v>
+      </c>
+      <c r="I36" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="J36" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="K36" s="11"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="14">
+        <f>M34+7</f>
+        <v>44856</v>
+      </c>
+      <c r="N36" s="15">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="O36" s="15">
+        <v>0.5625</v>
+      </c>
+      <c r="Q36" s="9">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="R36" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="S36" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="T36" s="9">
+        <v>50</v>
+      </c>
+      <c r="U36" s="9">
+        <v>2</v>
+      </c>
+      <c r="V36" s="9"/>
+    </row>
+    <row r="37" spans="7:22" x14ac:dyDescent="0.2">
+      <c r="G37">
+        <v>36</v>
+      </c>
+      <c r="H37" s="11">
+        <v>3</v>
+      </c>
+      <c r="I37" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="J37" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="K37" s="11"/>
+      <c r="L37" s="11"/>
+      <c r="M37" s="14">
+        <f>M36+1</f>
+        <v>44857</v>
+      </c>
+      <c r="N37" s="15">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="O37" s="15">
+        <v>0.5625</v>
+      </c>
+      <c r="Q37" s="9">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="R37" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="S37" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="T37" s="9">
+        <v>50</v>
+      </c>
+      <c r="U37" s="9">
+        <v>2</v>
+      </c>
+      <c r="V37" s="9"/>
+    </row>
+    <row r="38" spans="7:22" x14ac:dyDescent="0.2">
+      <c r="G38">
+        <v>37</v>
+      </c>
+      <c r="H38" s="11">
+        <v>3</v>
+      </c>
+      <c r="I38" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="J38" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="K38" s="11"/>
+      <c r="L38" s="11"/>
+      <c r="M38" s="14">
+        <f>M36+7</f>
+        <v>44863</v>
+      </c>
+      <c r="N38" s="15">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="O38" s="15">
+        <v>0.5625</v>
+      </c>
+      <c r="Q38" s="9">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="R38" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="S38" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="T38" s="9">
+        <v>115</v>
+      </c>
+      <c r="U38" s="9">
+        <v>2</v>
+      </c>
+      <c r="V38" s="9"/>
+    </row>
+    <row r="39" spans="7:22" x14ac:dyDescent="0.2">
+      <c r="G39">
+        <v>38</v>
+      </c>
+      <c r="H39" s="11">
+        <v>3</v>
+      </c>
+      <c r="I39" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="J39" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="K39" s="11"/>
+      <c r="L39" s="11"/>
+      <c r="M39" s="14">
+        <f>M38+1</f>
+        <v>44864</v>
+      </c>
+      <c r="N39" s="15">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="O39" s="15">
+        <v>0.5625</v>
+      </c>
+      <c r="Q39" s="9">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="R39" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="S39" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="T39" s="9">
+        <v>95</v>
+      </c>
+      <c r="U39" s="9">
+        <v>2</v>
+      </c>
+      <c r="V39" s="9"/>
+    </row>
+    <row r="40" spans="7:22" x14ac:dyDescent="0.2">
+      <c r="G40">
+        <v>39</v>
+      </c>
+      <c r="H40" s="11">
+        <v>3</v>
+      </c>
+      <c r="I40" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="J40" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="K40" s="11"/>
+      <c r="L40" s="11"/>
+      <c r="M40" s="14">
+        <f>M38+7</f>
+        <v>44870</v>
+      </c>
+      <c r="N40" s="15">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="O40" s="15">
+        <v>0.5625</v>
+      </c>
+      <c r="Q40" s="9">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="R40" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="S40" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="T40" s="9">
+        <v>115</v>
+      </c>
+      <c r="U40" s="9">
+        <v>2</v>
+      </c>
+      <c r="V40" s="9"/>
+    </row>
+    <row r="41" spans="7:22" x14ac:dyDescent="0.2">
+      <c r="G41">
+        <v>40</v>
+      </c>
+      <c r="H41" s="11">
+        <v>3</v>
+      </c>
+      <c r="I41" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="J41" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="K41" s="11"/>
+      <c r="L41" s="11"/>
+      <c r="M41" s="14">
+        <f>M40+1</f>
+        <v>44871</v>
+      </c>
+      <c r="N41" s="15">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="O41" s="15">
+        <v>0.5625</v>
+      </c>
+      <c r="Q41" s="9">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="R41" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="S41" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="T41" s="9">
+        <v>85</v>
+      </c>
+      <c r="U41" s="9">
+        <v>2</v>
+      </c>
+      <c r="V41" s="9"/>
+    </row>
+    <row r="42" spans="7:22" x14ac:dyDescent="0.2">
+      <c r="G42" s="16">
+        <v>41</v>
+      </c>
+      <c r="H42" s="17">
+        <v>3</v>
+      </c>
+      <c r="I42" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="J42" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="K42" s="17"/>
+      <c r="L42" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="M42" s="19">
+        <f>M30+1</f>
+        <v>44836</v>
+      </c>
+      <c r="N42" s="20">
+        <v>0.3125</v>
+      </c>
+      <c r="O42" s="20">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="Q42" s="9">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="R42" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="S42" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="T42" s="9">
+        <v>115</v>
+      </c>
+      <c r="U42" s="9">
+        <v>2</v>
+      </c>
+      <c r="V42" s="9"/>
+    </row>
+    <row r="43" spans="7:22" x14ac:dyDescent="0.2">
+      <c r="G43">
+        <v>42</v>
+      </c>
+      <c r="H43" s="11">
+        <v>3</v>
+      </c>
+      <c r="I43" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="J43" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="K43" s="11"/>
+      <c r="L43" s="11"/>
+      <c r="M43" s="14">
+        <f>M42+28</f>
+        <v>44864</v>
+      </c>
+      <c r="N43" s="15">
+        <v>0.3125</v>
+      </c>
+      <c r="O43" s="15">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="Q43" s="9">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="R43" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="S43" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="T43" s="9">
+        <v>85</v>
+      </c>
+      <c r="U43" s="9">
+        <v>2</v>
+      </c>
+      <c r="V43" s="9"/>
+    </row>
+    <row r="44" spans="7:22" x14ac:dyDescent="0.2">
+      <c r="G44">
+        <v>43</v>
+      </c>
+      <c r="H44" s="11">
+        <v>3</v>
+      </c>
+      <c r="I44" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="J44" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="K44" s="11"/>
+      <c r="L44" s="11"/>
+      <c r="M44" s="14">
+        <f>M43+35</f>
+        <v>44899</v>
+      </c>
+      <c r="N44" s="15">
+        <v>0.3125</v>
+      </c>
+      <c r="O44" s="15">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="Q44" s="9">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="R44" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="S44" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="T44" s="9">
+        <v>25</v>
+      </c>
+      <c r="U44" s="9">
+        <v>3</v>
+      </c>
+      <c r="V44" s="9"/>
+    </row>
+    <row r="45" spans="7:22" x14ac:dyDescent="0.2">
+      <c r="G45">
+        <v>44</v>
+      </c>
+      <c r="H45" s="11">
+        <v>3</v>
+      </c>
+      <c r="I45" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="J45" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="K45" s="11"/>
+      <c r="L45" s="11"/>
+      <c r="M45" s="14">
+        <f t="shared" ref="M45" si="6">M44+28</f>
+        <v>44927</v>
+      </c>
+      <c r="N45" s="15">
+        <v>0.3125</v>
+      </c>
+      <c r="O45" s="15">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="Q45" s="9">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="R45" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="S45" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="T45" s="9">
+        <v>25</v>
+      </c>
+      <c r="U45" s="9">
+        <v>3</v>
+      </c>
+      <c r="V45" s="9"/>
+    </row>
+    <row r="46" spans="7:22" x14ac:dyDescent="0.2">
+      <c r="G46">
+        <v>45</v>
+      </c>
+      <c r="H46" s="11">
+        <v>3</v>
+      </c>
+      <c r="I46" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="J46" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="K46" s="11"/>
+      <c r="L46" s="11"/>
+      <c r="M46" s="14">
+        <f>M45+35</f>
+        <v>44962</v>
+      </c>
+      <c r="N46" s="15">
+        <v>0.3125</v>
+      </c>
+      <c r="O46" s="15">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="Q46" s="9">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="R46" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="S46" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="T46" s="9">
+        <v>25</v>
+      </c>
+      <c r="U46" s="9">
+        <v>3</v>
+      </c>
+      <c r="V46" s="9"/>
+    </row>
+    <row r="47" spans="7:22" x14ac:dyDescent="0.2">
+      <c r="Q47" s="9">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="R47" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="S47" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="T47" s="9">
+        <v>25</v>
+      </c>
+      <c r="U47" s="9">
+        <v>3</v>
+      </c>
+      <c r="V47" s="9"/>
+    </row>
+    <row r="48" spans="7:22" x14ac:dyDescent="0.2">
+      <c r="Q48" s="9">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="R48" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="S48" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="T48" s="9">
+        <v>40</v>
+      </c>
+      <c r="U48" s="9">
+        <v>3</v>
+      </c>
+      <c r="V48" s="9"/>
+    </row>
+    <row r="49" spans="17:22" x14ac:dyDescent="0.2">
+      <c r="Q49" s="9">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="R49" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="S49" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="T49" s="9">
+        <v>40</v>
+      </c>
+      <c r="U49" s="9">
+        <v>3</v>
+      </c>
+      <c r="V49" s="9"/>
+    </row>
+    <row r="50" spans="17:22" x14ac:dyDescent="0.2">
+      <c r="Q50" s="9">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="R50" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="S50" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="T50" s="9">
+        <v>40</v>
+      </c>
+      <c r="U50" s="9">
+        <v>3</v>
+      </c>
+      <c r="V50" s="9"/>
+    </row>
+    <row r="51" spans="17:22" x14ac:dyDescent="0.2">
+      <c r="Q51" s="9">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="R51" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="S51" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="T51" s="9">
+        <v>40</v>
+      </c>
+      <c r="U51" s="9">
+        <v>3</v>
+      </c>
+      <c r="V51" s="9"/>
+    </row>
+    <row r="52" spans="17:22" x14ac:dyDescent="0.2">
+      <c r="Q52" s="9">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="R52" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="S52" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="T52" s="9">
+        <v>40</v>
+      </c>
+      <c r="U52" s="9">
+        <v>3</v>
+      </c>
+      <c r="V52" s="9"/>
+    </row>
+    <row r="53" spans="17:22" x14ac:dyDescent="0.2">
+      <c r="Q53" s="9">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="R53" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="S53" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="T53" s="9">
+        <v>40</v>
+      </c>
+      <c r="U53" s="9">
+        <v>3</v>
+      </c>
+      <c r="V53" s="9"/>
+    </row>
+    <row r="54" spans="17:22" x14ac:dyDescent="0.2">
+      <c r="Q54" s="9">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="R54" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="S54" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="T54" s="9">
+        <v>45</v>
+      </c>
+      <c r="U54" s="9">
+        <v>3</v>
+      </c>
+      <c r="V54" s="9"/>
+    </row>
+    <row r="55" spans="17:22" x14ac:dyDescent="0.2">
+      <c r="Q55" s="9">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="R55" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="S55" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="T55" s="9">
+        <v>45</v>
+      </c>
+      <c r="U55" s="9">
+        <v>3</v>
+      </c>
+      <c r="V55" s="9"/>
+    </row>
+    <row r="56" spans="17:22" x14ac:dyDescent="0.2">
+      <c r="Q56" s="9">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="R56" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="S56" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="T56" s="9">
+        <v>45</v>
+      </c>
+      <c r="U56" s="9">
+        <v>3</v>
+      </c>
+      <c r="V56" s="9"/>
+    </row>
+    <row r="57" spans="17:22" x14ac:dyDescent="0.2">
+      <c r="Q57" s="9">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="R57" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="S57" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="T57" s="9">
+        <v>50</v>
+      </c>
+      <c r="U57" s="9">
+        <v>3</v>
+      </c>
+      <c r="V57" s="9"/>
+    </row>
+    <row r="58" spans="17:22" x14ac:dyDescent="0.2">
+      <c r="Q58" s="9">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="R58" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="S58" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="T58" s="9">
+        <v>50</v>
+      </c>
+      <c r="U58" s="9">
+        <v>3</v>
+      </c>
+      <c r="V58" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Got eventsBooking route to work
</commit_message>
<xml_diff>
--- a/seeds/Formulaic Seed generation.xlsx
+++ b/seeds/Formulaic Seed generation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reeveschragger/Documents/Bootcamp/Projects/Farmers-Market-Organiser/seeds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EEF60C2-1F52-5F48-9FA9-44BE27B77045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF08CDA-D5E6-5A42-91B9-D2CF6A4691D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16340" activeTab="2" xr2:uid="{E72EE37F-B9BE-8B4C-AF7C-D3608E94063D}"/>
   </bookViews>
@@ -246,18 +246,12 @@
     <t>Likely_Stall_ID</t>
   </si>
   <si>
-    <t>event_id</t>
-  </si>
-  <si>
     <t>stall_id</t>
   </si>
   <si>
     <t>lease_start</t>
   </si>
   <si>
-    <t>event_id(ikely)</t>
-  </si>
-  <si>
     <t>3days</t>
   </si>
   <si>
@@ -547,6 +541,12 @@
   </si>
   <si>
     <t>stallholder_id</t>
+  </si>
+  <si>
+    <t>events_id</t>
+  </si>
+  <si>
+    <t>events_id(ikely)</t>
   </si>
 </sst>
 </file>
@@ -2050,10 +2050,10 @@
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>168</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -3105,7 +3105,7 @@
   <dimension ref="A1:V58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3122,10 +3122,10 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G1" t="s">
-        <v>72</v>
+        <v>169</v>
       </c>
       <c r="H1" s="11" t="s">
         <v>3</v>
@@ -3166,10 +3166,10 @@
         <v>1</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K2" s="11"/>
       <c r="L2" s="11" t="s">
@@ -3203,16 +3203,16 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" t="s">
         <v>70</v>
       </c>
-      <c r="C3" t="s">
-        <v>71</v>
-      </c>
       <c r="D3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -3221,10 +3221,10 @@
         <v>1</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
@@ -3263,13 +3263,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G4">
         <v>3</v>
@@ -3278,10 +3278,10 @@
         <v>1</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K4" s="11"/>
       <c r="L4" s="11"/>
@@ -3320,13 +3320,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G5">
         <v>4</v>
@@ -3335,10 +3335,10 @@
         <v>1</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
@@ -3377,13 +3377,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G6">
         <v>5</v>
@@ -3392,10 +3392,10 @@
         <v>1</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
@@ -3435,13 +3435,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G7">
         <v>6</v>
@@ -3450,10 +3450,10 @@
         <v>1</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K7" s="11"/>
       <c r="L7" s="11"/>
@@ -3493,13 +3493,13 @@
         <v>41</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G8">
         <v>7</v>
@@ -3508,10 +3508,10 @@
         <v>1</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K8" s="11"/>
       <c r="L8" s="11"/>
@@ -3551,13 +3551,13 @@
         <v>42</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G9">
         <v>8</v>
@@ -3566,10 +3566,10 @@
         <v>1</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K9" s="11"/>
       <c r="L9" s="11"/>
@@ -3610,10 +3610,10 @@
         <v>1</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K10" s="11"/>
       <c r="L10" s="11"/>
@@ -3653,10 +3653,10 @@
         <v>1</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K11" s="11"/>
       <c r="L11" s="11"/>
@@ -3690,7 +3690,7 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G12">
         <v>11</v>
@@ -3699,10 +3699,10 @@
         <v>1</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K12" s="11"/>
       <c r="L12" s="11"/>
@@ -3736,13 +3736,13 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>168</v>
+      </c>
+      <c r="B13" t="s">
         <v>69</v>
       </c>
-      <c r="B13" t="s">
-        <v>70</v>
-      </c>
       <c r="C13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G13">
         <v>12</v>
@@ -3751,10 +3751,10 @@
         <v>1</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K13" s="11"/>
       <c r="L13" s="11"/>
@@ -3805,10 +3805,10 @@
         <v>1</v>
       </c>
       <c r="I14" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K14" s="11"/>
       <c r="L14" s="11"/>
@@ -3860,10 +3860,10 @@
         <v>1</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K15" s="11"/>
       <c r="L15" s="11"/>
@@ -3915,10 +3915,10 @@
         <v>1</v>
       </c>
       <c r="I16" s="13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J16" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K16" s="11"/>
       <c r="L16" s="11"/>
@@ -3970,10 +3970,10 @@
         <v>1</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="K17" s="11"/>
       <c r="L17" s="11"/>
@@ -4025,10 +4025,10 @@
         <v>1</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J18" s="11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K18" s="11"/>
       <c r="L18" s="11"/>
@@ -4080,10 +4080,10 @@
         <v>1</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J19" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K19" s="11"/>
       <c r="L19" s="11"/>
@@ -4135,10 +4135,10 @@
         <v>1</v>
       </c>
       <c r="I20" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J20" s="11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K20" s="11"/>
       <c r="L20" s="11"/>
@@ -4190,10 +4190,10 @@
         <v>1</v>
       </c>
       <c r="I21" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J21" s="11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="K21" s="11"/>
       <c r="L21" s="11"/>
@@ -4245,10 +4245,10 @@
         <v>2</v>
       </c>
       <c r="I22" s="18" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J22" s="17" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="K22" s="17"/>
       <c r="L22" s="17" t="s">
@@ -4301,10 +4301,10 @@
         <v>2</v>
       </c>
       <c r="I23" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J23" s="11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="K23" s="11"/>
       <c r="L23" s="11"/>
@@ -4354,10 +4354,10 @@
         <v>2</v>
       </c>
       <c r="I24" s="13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J24" s="11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K24" s="11"/>
       <c r="L24" s="11"/>
@@ -4407,10 +4407,10 @@
         <v>2</v>
       </c>
       <c r="I25" s="13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J25" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K25" s="11"/>
       <c r="L25" s="11"/>
@@ -4450,10 +4450,10 @@
         <v>2</v>
       </c>
       <c r="I26" s="13" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J26" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="K26" s="11"/>
       <c r="L26" s="11"/>
@@ -4493,10 +4493,10 @@
         <v>2</v>
       </c>
       <c r="I27" s="13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J27" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="K27" s="11"/>
       <c r="L27" s="11"/>
@@ -4536,10 +4536,10 @@
         <v>2</v>
       </c>
       <c r="I28" s="13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="J28" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K28" s="11"/>
       <c r="L28" s="11"/>
@@ -4579,10 +4579,10 @@
         <v>2</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J29" s="11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K29" s="11"/>
       <c r="L29" s="11"/>
@@ -4622,10 +4622,10 @@
         <v>2</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J30" s="11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K30" s="11"/>
       <c r="L30" s="11"/>
@@ -4665,10 +4665,10 @@
         <v>2</v>
       </c>
       <c r="I31" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J31" s="11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K31" s="11"/>
       <c r="L31" s="11"/>
@@ -4708,10 +4708,10 @@
         <v>2</v>
       </c>
       <c r="I32" s="13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J32" s="11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K32" s="11"/>
       <c r="L32" s="11"/>
@@ -4751,10 +4751,10 @@
         <v>2</v>
       </c>
       <c r="I33" s="13" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J33" s="11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="K33" s="11"/>
       <c r="L33" s="11"/>
@@ -4794,10 +4794,10 @@
         <v>3</v>
       </c>
       <c r="I34" s="13" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J34" s="11" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K34" s="11"/>
       <c r="L34" s="11"/>
@@ -4837,10 +4837,10 @@
         <v>3</v>
       </c>
       <c r="I35" s="13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J35" s="11" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="K35" s="11"/>
       <c r="L35" s="11"/>
@@ -4880,10 +4880,10 @@
         <v>3</v>
       </c>
       <c r="I36" s="13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="J36" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="K36" s="11"/>
       <c r="L36" s="11"/>
@@ -4923,10 +4923,10 @@
         <v>3</v>
       </c>
       <c r="I37" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J37" s="11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="K37" s="11"/>
       <c r="L37" s="11"/>
@@ -4966,10 +4966,10 @@
         <v>3</v>
       </c>
       <c r="I38" s="13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J38" s="11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="K38" s="11"/>
       <c r="L38" s="11"/>
@@ -5009,10 +5009,10 @@
         <v>3</v>
       </c>
       <c r="I39" s="13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J39" s="11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K39" s="11"/>
       <c r="L39" s="11"/>
@@ -5052,10 +5052,10 @@
         <v>3</v>
       </c>
       <c r="I40" s="13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J40" s="11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="K40" s="11"/>
       <c r="L40" s="11"/>
@@ -5095,10 +5095,10 @@
         <v>3</v>
       </c>
       <c r="I41" s="13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J41" s="11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K41" s="11"/>
       <c r="L41" s="11"/>
@@ -5138,10 +5138,10 @@
         <v>3</v>
       </c>
       <c r="I42" s="18" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J42" s="17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="K42" s="17"/>
       <c r="L42" s="17" t="s">
@@ -5183,10 +5183,10 @@
         <v>3</v>
       </c>
       <c r="I43" s="13" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J43" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="K43" s="11"/>
       <c r="L43" s="11"/>
@@ -5226,10 +5226,10 @@
         <v>3</v>
       </c>
       <c r="I44" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J44" s="11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="K44" s="11"/>
       <c r="L44" s="11"/>
@@ -5269,10 +5269,10 @@
         <v>3</v>
       </c>
       <c r="I45" s="13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="J45" s="11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="K45" s="11"/>
       <c r="L45" s="11"/>
@@ -5312,10 +5312,10 @@
         <v>3</v>
       </c>
       <c r="I46" s="13" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J46" s="11" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="K46" s="11"/>
       <c r="L46" s="11"/>

</xml_diff>